<commit_message>
18 tescase for osprey e2e
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Osprey_EMEA/OSPEMEA_E2E_orderDetails.xlsx
+++ b/src/test/resources/TestData/Osprey_EMEA/OSPEMEA_E2E_orderDetails.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F398A60-FF28-4847-9BFC-6AF9BB72615A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF36770E-376C-4A66-BE08-B9ADA19B99D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="13" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1764" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1787" uniqueCount="488">
   <si>
     <t>UserName</t>
   </si>
@@ -1496,6 +1496,39 @@
   </si>
   <si>
     <t>Narra</t>
+  </si>
+  <si>
+    <t>SKU-10000645 -2QTY</t>
+  </si>
+  <si>
+    <t>SKU-10002926 -2QTY CHE</t>
+  </si>
+  <si>
+    <t>Sweden-fr Address</t>
+  </si>
+  <si>
+    <t>Piazza Indipendenza 5</t>
+  </si>
+  <si>
+    <t>Chiasso</t>
+  </si>
+  <si>
+    <t>Ticino</t>
+  </si>
+  <si>
+    <t>6830</t>
+  </si>
+  <si>
+    <t>2AZ62B26X4675X42C96S</t>
+  </si>
+  <si>
+    <t>10002926</t>
+  </si>
+  <si>
+    <t>CHE SKU-10002926</t>
+  </si>
+  <si>
+    <t>Daylite®</t>
   </si>
 </sst>
 </file>
@@ -1677,7 +1710,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1726,6 +1759,12 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5893,12 +5932,12 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
-  <dimension ref="A1:AT49"/>
+  <dimension ref="A1:AT54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomLeft" activeCell="AH39" sqref="AH39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6960,43 +6999,38 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>391</v>
-      </c>
-      <c r="AE39" s="29" t="s">
-        <v>397</v>
+        <v>478</v>
+      </c>
+      <c r="AE39" s="36" t="s">
+        <v>487</v>
       </c>
       <c r="AF39" t="s">
-        <v>398</v>
+        <v>191</v>
+      </c>
+      <c r="AH39" s="36" t="s">
+        <v>487</v>
       </c>
       <c r="AI39" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="40" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>414</v>
-      </c>
-      <c r="AE40" s="29" t="s">
-        <v>415</v>
-      </c>
-      <c r="AF40" s="34" t="s">
-        <v>416</v>
-      </c>
-      <c r="AI40" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="41" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+        <v>486</v>
+      </c>
+      <c r="AE40" s="37" t="s">
+        <v>485</v>
+      </c>
+      <c r="AI40" s="5"/>
+    </row>
+    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>419</v>
-      </c>
-      <c r="AE41" s="29" t="s">
-        <v>417</v>
-      </c>
-      <c r="AF41" s="34" t="s">
-        <v>418</v>
+        <v>477</v>
+      </c>
+      <c r="AE41" s="36" t="s">
+        <v>387</v>
       </c>
       <c r="AI41" s="5" t="s">
         <v>122</v>
@@ -7004,13 +7038,13 @@
     </row>
     <row r="42" spans="1:46" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>420</v>
+        <v>391</v>
       </c>
       <c r="AE42" s="29" t="s">
-        <v>417</v>
-      </c>
-      <c r="AF42" s="34" t="s">
-        <v>418</v>
+        <v>397</v>
+      </c>
+      <c r="AF42" t="s">
+        <v>398</v>
       </c>
       <c r="AI42" s="5" t="s">
         <v>188</v>
@@ -7018,7 +7052,7 @@
     </row>
     <row r="43" spans="1:46" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="AE43" s="29" t="s">
         <v>415</v>
@@ -7027,139 +7061,103 @@
         <v>416</v>
       </c>
       <c r="AI43" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>419</v>
+      </c>
+      <c r="AE44" s="29" t="s">
+        <v>417</v>
+      </c>
+      <c r="AF44" s="34" t="s">
+        <v>418</v>
+      </c>
+      <c r="AI44" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>420</v>
+      </c>
+      <c r="AE45" s="29" t="s">
+        <v>417</v>
+      </c>
+      <c r="AF45" s="34" t="s">
+        <v>418</v>
+      </c>
+      <c r="AI45" s="5" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="46" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>421</v>
+      </c>
+      <c r="AE46" s="29" t="s">
+        <v>415</v>
+      </c>
+      <c r="AF46" s="34" t="s">
+        <v>416</v>
+      </c>
+      <c r="AI46" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="47" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>428</v>
       </c>
-      <c r="AE44" s="33" t="s">
+      <c r="AE47" s="33" t="s">
         <v>431</v>
       </c>
-      <c r="AF44" s="34" t="s">
+      <c r="AF47" s="34" t="s">
         <v>429</v>
       </c>
-      <c r="AI44" s="5" t="s">
+      <c r="AI47" s="5" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="48" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>392</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="R45" t="s">
+      <c r="R48" t="s">
         <v>475</v>
       </c>
-      <c r="S45" t="s">
+      <c r="S48" t="s">
         <v>476</v>
       </c>
-      <c r="T45" t="s">
+      <c r="T48" t="s">
         <v>393</v>
       </c>
-      <c r="U45" t="s">
+      <c r="U48" t="s">
         <v>394</v>
       </c>
-      <c r="V45" t="s">
+      <c r="V48" t="s">
         <v>396</v>
       </c>
-      <c r="W45" s="5" t="s">
+      <c r="W48" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="X45" s="5" t="s">
+      <c r="X48" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="49" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>408</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="R46" t="s">
-        <v>475</v>
-      </c>
-      <c r="S46" t="s">
-        <v>476</v>
-      </c>
-      <c r="T46" t="s">
-        <v>405</v>
-      </c>
-      <c r="U46" t="s">
-        <v>406</v>
-      </c>
-      <c r="V46" t="s">
-        <v>404</v>
-      </c>
-      <c r="W46" s="31" t="s">
-        <v>407</v>
-      </c>
-      <c r="X46" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>409</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="R47" t="s">
-        <v>475</v>
-      </c>
-      <c r="S47" t="s">
-        <v>476</v>
-      </c>
-      <c r="T47" s="32" t="s">
-        <v>410</v>
-      </c>
-      <c r="U47" s="32" t="s">
-        <v>411</v>
-      </c>
-      <c r="V47" s="33" t="s">
-        <v>413</v>
-      </c>
-      <c r="W47" s="31" t="s">
-        <v>412</v>
-      </c>
-      <c r="X47" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="48" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>401</v>
-      </c>
-      <c r="AO48" s="30" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>422</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>278</v>
@@ -7176,20 +7174,141 @@
       <c r="S49" t="s">
         <v>476</v>
       </c>
-      <c r="T49" s="35" t="s">
+      <c r="T49" t="s">
+        <v>405</v>
+      </c>
+      <c r="U49" t="s">
+        <v>406</v>
+      </c>
+      <c r="V49" t="s">
+        <v>404</v>
+      </c>
+      <c r="W49" s="31" t="s">
+        <v>407</v>
+      </c>
+      <c r="X49" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>409</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="R50" t="s">
+        <v>475</v>
+      </c>
+      <c r="S50" t="s">
+        <v>476</v>
+      </c>
+      <c r="T50" s="32" t="s">
+        <v>410</v>
+      </c>
+      <c r="U50" s="32" t="s">
+        <v>411</v>
+      </c>
+      <c r="V50" s="33" t="s">
+        <v>413</v>
+      </c>
+      <c r="W50" s="31" t="s">
+        <v>412</v>
+      </c>
+      <c r="X50" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>401</v>
+      </c>
+      <c r="AO51" s="30" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="52" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>433</v>
+      </c>
+      <c r="AO52" s="30" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>422</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="R53" t="s">
+        <v>475</v>
+      </c>
+      <c r="S53" t="s">
+        <v>476</v>
+      </c>
+      <c r="T53" s="35" t="s">
         <v>425</v>
       </c>
-      <c r="U49" s="35" t="s">
+      <c r="U53" s="35" t="s">
         <v>426</v>
       </c>
-      <c r="V49" s="33" t="s">
+      <c r="V53" s="33" t="s">
         <v>430</v>
       </c>
-      <c r="W49" s="35" t="s">
+      <c r="W53" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="X49" s="5" t="s">
+      <c r="X53" s="5" t="s">
         <v>423</v>
+      </c>
+    </row>
+    <row r="54" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>479</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="R54" t="s">
+        <v>475</v>
+      </c>
+      <c r="S54" t="s">
+        <v>476</v>
+      </c>
+      <c r="T54" t="s">
+        <v>480</v>
+      </c>
+      <c r="U54" t="s">
+        <v>481</v>
+      </c>
+      <c r="V54" t="s">
+        <v>482</v>
+      </c>
+      <c r="W54" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="X54" s="5" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -7221,21 +7340,24 @@
     <hyperlink ref="B11" r:id="rId25" xr:uid="{00000000-0004-0000-1600-000018000000}"/>
     <hyperlink ref="B15" r:id="rId26" xr:uid="{00000000-0004-0000-1600-000019000000}"/>
     <hyperlink ref="C35" r:id="rId27" xr:uid="{1864C442-0D98-42E4-A5FA-B81EFAA05600}"/>
-    <hyperlink ref="B45" r:id="rId28" display="testersemail.278@gmail.com" xr:uid="{34BD3CEC-6340-4CBD-96DC-8D004250BF84}"/>
-    <hyperlink ref="C45" r:id="rId29" display="testersemail.278@gmail.com" xr:uid="{F1625DAF-2FCD-401E-B451-0BDE8A534010}"/>
-    <hyperlink ref="D45" r:id="rId30" display="testersemail.278@gmail.com" xr:uid="{07702DCB-4B62-4824-BB8A-83439182C0EA}"/>
-    <hyperlink ref="B46" r:id="rId31" display="testersemail.278@gmail.com" xr:uid="{5B1965CC-AC91-4E74-81AB-F5894D8C2D9D}"/>
-    <hyperlink ref="C46" r:id="rId32" display="testersemail.278@gmail.com" xr:uid="{41C8C86C-6596-41A3-B56B-A8BC6862F5E2}"/>
-    <hyperlink ref="D46" r:id="rId33" display="testersemail.278@gmail.com" xr:uid="{6A001A27-2D56-448C-93B5-920CBED417DB}"/>
-    <hyperlink ref="B47" r:id="rId34" display="testersemail.278@gmail.com" xr:uid="{E91B6625-1005-4D68-8C77-C24DDB033C2B}"/>
-    <hyperlink ref="C47" r:id="rId35" display="testersemail.278@gmail.com" xr:uid="{015DE811-F050-4B71-96A8-193BA2EE4365}"/>
-    <hyperlink ref="D47" r:id="rId36" display="testersemail.278@gmail.com" xr:uid="{6A56F90F-8F22-4C03-B66D-47272E68A409}"/>
-    <hyperlink ref="B49" r:id="rId37" display="testersemail.278@gmail.com" xr:uid="{6ECC3E7A-0650-471A-8118-361B581591B2}"/>
-    <hyperlink ref="C49" r:id="rId38" display="testersemail.278@gmail.com" xr:uid="{FFDC6FD4-A6DF-4655-B604-131C2FEC8FCA}"/>
-    <hyperlink ref="D49" r:id="rId39" display="testersemail.278@gmail.com" xr:uid="{E68CD518-C7DB-4D2A-BFE5-92473B1B7D82}"/>
+    <hyperlink ref="B48" r:id="rId28" display="testersemail.278@gmail.com" xr:uid="{34BD3CEC-6340-4CBD-96DC-8D004250BF84}"/>
+    <hyperlink ref="C48" r:id="rId29" display="testersemail.278@gmail.com" xr:uid="{F1625DAF-2FCD-401E-B451-0BDE8A534010}"/>
+    <hyperlink ref="D48" r:id="rId30" display="testersemail.278@gmail.com" xr:uid="{07702DCB-4B62-4824-BB8A-83439182C0EA}"/>
+    <hyperlink ref="B49" r:id="rId31" display="testersemail.278@gmail.com" xr:uid="{5B1965CC-AC91-4E74-81AB-F5894D8C2D9D}"/>
+    <hyperlink ref="C49" r:id="rId32" display="testersemail.278@gmail.com" xr:uid="{41C8C86C-6596-41A3-B56B-A8BC6862F5E2}"/>
+    <hyperlink ref="D49" r:id="rId33" display="testersemail.278@gmail.com" xr:uid="{6A001A27-2D56-448C-93B5-920CBED417DB}"/>
+    <hyperlink ref="B50" r:id="rId34" display="testersemail.278@gmail.com" xr:uid="{E91B6625-1005-4D68-8C77-C24DDB033C2B}"/>
+    <hyperlink ref="C50" r:id="rId35" display="testersemail.278@gmail.com" xr:uid="{015DE811-F050-4B71-96A8-193BA2EE4365}"/>
+    <hyperlink ref="D50" r:id="rId36" display="testersemail.278@gmail.com" xr:uid="{6A56F90F-8F22-4C03-B66D-47272E68A409}"/>
+    <hyperlink ref="B53" r:id="rId37" display="testersemail.278@gmail.com" xr:uid="{6ECC3E7A-0650-471A-8118-361B581591B2}"/>
+    <hyperlink ref="C53" r:id="rId38" display="testersemail.278@gmail.com" xr:uid="{FFDC6FD4-A6DF-4655-B604-131C2FEC8FCA}"/>
+    <hyperlink ref="D53" r:id="rId39" display="testersemail.278@gmail.com" xr:uid="{E68CD518-C7DB-4D2A-BFE5-92473B1B7D82}"/>
+    <hyperlink ref="B54" r:id="rId40" display="testersemail.278@gmail.com" xr:uid="{C068F1CE-D006-4174-81C1-E2703766A79B}"/>
+    <hyperlink ref="C54" r:id="rId41" display="testersemail.278@gmail.com" xr:uid="{2393F234-B92D-48CB-B748-088EB5B8D9F0}"/>
+    <hyperlink ref="D54" r:id="rId42" display="testersemail.278@gmail.com" xr:uid="{EB4696D1-B300-4BCB-8F2F-4D7BB5228026}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId40"/>
+  <pageSetup orientation="portrait" r:id="rId43"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
18 testcase changes for osprey us
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Osprey_EMEA/OSPEMEA_E2E_orderDetails.xlsx
+++ b/src/test/resources/TestData/Osprey_EMEA/OSPEMEA_E2E_orderDetails.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF36770E-376C-4A66-BE08-B9ADA19B99D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2B4251-673B-4526-8D09-30B66E679887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="13" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1787" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1789" uniqueCount="490">
   <si>
     <t>UserName</t>
   </si>
@@ -1529,6 +1529,12 @@
   </si>
   <si>
     <t>Daylite®</t>
+  </si>
+  <si>
+    <t>CHE groundshipping</t>
+  </si>
+  <si>
+    <t>Standard Delivery (2-7 Days)</t>
   </si>
 </sst>
 </file>
@@ -5932,12 +5938,12 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
-  <dimension ref="A1:AT54"/>
+  <dimension ref="A1:AT55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="AH39" sqref="AH39"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6206,105 +6212,97 @@
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>383</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="9"/>
-      <c r="M5" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="N5" s="2"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="2"/>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
-      <c r="AE5" s="5"/>
-      <c r="AF5" s="7"/>
-      <c r="AK5" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="AL5" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="AM5">
-        <v>123</v>
+        <v>488</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="AJ5" s="5" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>261</v>
-      </c>
-      <c r="M6" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="9"/>
+      <c r="M6" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="AJ6" t="s">
-        <v>262</v>
+      <c r="N6" s="2"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="2"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="7"/>
+      <c r="AK6" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="AL6" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM6">
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>99</v>
-      </c>
-      <c r="M7" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="AK7" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="AL7" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="AM7">
-        <v>123</v>
+      <c r="AJ7" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>102</v>
-      </c>
-      <c r="M8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M8" s="5" t="s">
         <v>204</v>
       </c>
       <c r="AK8" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="AL8" s="7" t="s">
         <v>101</v>
       </c>
       <c r="AM8">
-        <v>1234</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>104</v>
-      </c>
-      <c r="M9" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="M9" s="2" t="s">
         <v>204</v>
       </c>
       <c r="AK9" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="AL9" s="7" t="s">
         <v>101</v>
       </c>
       <c r="AM9">
-        <v>123</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>106</v>
-      </c>
-      <c r="M10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M10" s="5" t="s">
         <v>204</v>
       </c>
       <c r="AK10" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AL10" s="7" t="s">
         <v>101</v>
@@ -6315,214 +6313,173 @@
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="M11" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" t="s">
-        <v>45</v>
-      </c>
-      <c r="S11" t="s">
-        <v>46</v>
+      <c r="AK11" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL11" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM11">
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>74</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="M12" s="2" t="s">
+      <c r="E12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="5" t="s">
         <v>204</v>
       </c>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
       <c r="R12" t="s">
         <v>45</v>
       </c>
       <c r="S12" t="s">
-        <v>73</v>
-      </c>
-      <c r="T12" s="2"/>
-      <c r="U12" t="s">
-        <v>176</v>
-      </c>
-      <c r="V12" t="s">
-        <v>175</v>
-      </c>
-      <c r="W12" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="X12" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y12" s="5"/>
-      <c r="Z12" s="5"/>
-      <c r="AA12" s="5"/>
-      <c r="AB12" s="5"/>
-      <c r="AC12" s="5"/>
-      <c r="AD12" s="5"/>
-      <c r="AF12" s="5"/>
-      <c r="AG12" s="5"/>
-      <c r="AH12" s="5"/>
-      <c r="AI12" s="5"/>
+        <v>46</v>
+      </c>
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>112</v>
-      </c>
-      <c r="M13" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="M13" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="AK13" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="AL13" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="AM13">
-        <v>12</v>
-      </c>
+      <c r="R13" t="s">
+        <v>45</v>
+      </c>
+      <c r="S13" t="s">
+        <v>73</v>
+      </c>
+      <c r="T13" s="2"/>
+      <c r="U13" t="s">
+        <v>176</v>
+      </c>
+      <c r="V13" t="s">
+        <v>175</v>
+      </c>
+      <c r="W13" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="X13" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="5"/>
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="5"/>
+      <c r="AF13" s="5"/>
+      <c r="AG13" s="5"/>
+      <c r="AH13" s="5"/>
+      <c r="AI13" s="5"/>
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>141</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="M14" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="M14" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="AF14" s="5"/>
-      <c r="AG14" s="5"/>
+      <c r="AK14" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="AL14" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="AM14">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>144</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>294</v>
+        <v>141</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>278</v>
+        <v>143</v>
       </c>
       <c r="D15" s="2"/>
-      <c r="E15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="5" t="s">
+      <c r="E15" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="M15" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="AF15" s="5"/>
+      <c r="AG15" s="5"/>
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>146</v>
-      </c>
-      <c r="M16" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="R16" t="s">
-        <v>46</v>
-      </c>
-      <c r="S16" t="s">
-        <v>92</v>
-      </c>
-      <c r="T16" t="s">
-        <v>243</v>
-      </c>
-      <c r="U16" t="s">
-        <v>244</v>
-      </c>
-      <c r="V16" t="s">
-        <v>245</v>
-      </c>
-      <c r="W16" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="X16" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y16" s="5"/>
-      <c r="Z16" s="5"/>
-      <c r="AA16" s="5"/>
-      <c r="AB16" s="5"/>
-      <c r="AC16" s="5"/>
-      <c r="AD16" s="5"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>151</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="M17" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
       <c r="R17" t="s">
         <v>46</v>
       </c>
@@ -6530,16 +6487,16 @@
         <v>92</v>
       </c>
       <c r="T17" t="s">
-        <v>152</v>
+        <v>243</v>
       </c>
       <c r="U17" t="s">
-        <v>153</v>
+        <v>244</v>
       </c>
       <c r="V17" t="s">
-        <v>154</v>
+        <v>245</v>
       </c>
       <c r="W17" s="5" t="s">
-        <v>155</v>
+        <v>246</v>
       </c>
       <c r="X17" s="5" t="s">
         <v>93</v>
@@ -6550,21 +6507,18 @@
       <c r="AB17" s="5"/>
       <c r="AC17" s="5"/>
       <c r="AD17" s="5"/>
-      <c r="AG17" s="5"/>
-      <c r="AI17" s="5"/>
-      <c r="AJ17" s="7"/>
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>156</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="D18" s="10"/>
+        <v>151</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D18" s="2"/>
       <c r="E18" s="9" t="s">
         <v>47</v>
       </c>
@@ -6577,7 +6531,7 @@
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
-      <c r="M18" s="2" t="s">
+      <c r="M18" s="5" t="s">
         <v>204</v>
       </c>
       <c r="N18" s="9"/>
@@ -6591,16 +6545,16 @@
         <v>92</v>
       </c>
       <c r="T18" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="U18" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="V18" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="W18" s="5" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="X18" s="5" t="s">
         <v>93</v>
@@ -6611,130 +6565,180 @@
       <c r="AB18" s="5"/>
       <c r="AC18" s="5"/>
       <c r="AD18" s="5"/>
-      <c r="AE18" s="5"/>
+      <c r="AG18" s="5"/>
+      <c r="AI18" s="5"/>
+      <c r="AJ18" s="7"/>
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>166</v>
-      </c>
-      <c r="M19" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="AE19" t="s">
-        <v>263</v>
-      </c>
-      <c r="AG19" s="5"/>
-      <c r="AI19" s="5" t="s">
-        <v>72</v>
-      </c>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" t="s">
+        <v>46</v>
+      </c>
+      <c r="S19" t="s">
+        <v>92</v>
+      </c>
+      <c r="T19" t="s">
+        <v>158</v>
+      </c>
+      <c r="U19" t="s">
+        <v>159</v>
+      </c>
+      <c r="V19" t="s">
+        <v>160</v>
+      </c>
+      <c r="W19" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="X19" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="5"/>
+      <c r="AC19" s="5"/>
+      <c r="AD19" s="5"/>
+      <c r="AE19" s="5"/>
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>178</v>
-      </c>
-      <c r="M20" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="M20" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="AJ20" s="5" t="s">
-        <v>299</v>
+      <c r="AE20" t="s">
+        <v>263</v>
+      </c>
+      <c r="AG20" s="5"/>
+      <c r="AI20" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>186</v>
-      </c>
-      <c r="M21" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="M21" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="N21" t="s">
-        <v>208</v>
-      </c>
-      <c r="R21" t="s">
-        <v>46</v>
-      </c>
-      <c r="S21" t="s">
-        <v>92</v>
-      </c>
-      <c r="AN21" t="s">
-        <v>187</v>
+      <c r="AJ21" s="5" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>91</v>
-      </c>
-      <c r="M22" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="M22" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="AI22" s="5" t="s">
-        <v>72</v>
+      <c r="N22" t="s">
+        <v>208</v>
+      </c>
+      <c r="R22" t="s">
+        <v>46</v>
+      </c>
+      <c r="S22" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN22" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>201</v>
-      </c>
-      <c r="G23" t="s">
-        <v>201</v>
-      </c>
-      <c r="H23" t="s">
-        <v>264</v>
-      </c>
-      <c r="M23" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="M23" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="Q23" t="s">
-        <v>265</v>
+      <c r="AI23" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="G24" t="s">
+        <v>201</v>
+      </c>
+      <c r="H24" t="s">
+        <v>264</v>
       </c>
       <c r="M24" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="N24" t="s">
-        <v>375</v>
-      </c>
-      <c r="O24" s="5" t="s">
-        <v>350</v>
-      </c>
-      <c r="P24" s="5" t="s">
-        <v>207</v>
+      <c r="Q24" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>230</v>
+        <v>203</v>
       </c>
       <c r="M25" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="AO25" t="s">
-        <v>242</v>
-      </c>
-      <c r="AP25" t="s">
-        <v>242</v>
-      </c>
-      <c r="AQ25" t="s">
-        <v>229</v>
+      <c r="N25" t="s">
+        <v>375</v>
+      </c>
+      <c r="O25" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="P25" s="5" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>253</v>
+        <v>230</v>
       </c>
       <c r="M26" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="AE26" t="s">
-        <v>252</v>
+      <c r="AO26" t="s">
+        <v>242</v>
+      </c>
+      <c r="AP26" t="s">
+        <v>242</v>
+      </c>
+      <c r="AQ26" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="M27" s="5" t="s">
         <v>204</v>
@@ -6745,124 +6749,111 @@
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>256</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D28" s="10"/>
+        <v>255</v>
+      </c>
       <c r="M28" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
-      <c r="R28" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="S28" t="s">
-        <v>45</v>
-      </c>
-      <c r="T28" t="s">
-        <v>243</v>
-      </c>
-      <c r="U28" t="s">
-        <v>244</v>
-      </c>
-      <c r="V28" t="s">
-        <v>245</v>
-      </c>
-      <c r="W28" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="X28" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="Y28" s="5"/>
-      <c r="Z28" s="5"/>
-      <c r="AA28" s="5">
-        <v>888888</v>
-      </c>
-      <c r="AB28" s="5"/>
-      <c r="AC28" s="5"/>
-      <c r="AD28" s="5"/>
-      <c r="AE28" s="5"/>
-      <c r="AF28" s="24" t="s">
-        <v>258</v>
-      </c>
-      <c r="AH28" s="5"/>
-      <c r="AI28" s="5"/>
-      <c r="AJ28" s="5"/>
-      <c r="AK28" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="AL28" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="AM28" s="5">
-        <v>123</v>
-      </c>
-      <c r="AN28" s="7"/>
+      <c r="AE28" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>115</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="K29" t="s">
-        <v>45</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>278</v>
-      </c>
+        <v>256</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="10"/>
       <c r="M29" s="5" t="s">
         <v>204</v>
       </c>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="S29" t="s">
+        <v>45</v>
+      </c>
+      <c r="T29" t="s">
+        <v>243</v>
+      </c>
+      <c r="U29" t="s">
+        <v>244</v>
+      </c>
+      <c r="V29" t="s">
+        <v>245</v>
+      </c>
+      <c r="W29" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="X29" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="5"/>
+      <c r="AA29" s="5">
+        <v>888888</v>
+      </c>
+      <c r="AB29" s="5"/>
+      <c r="AC29" s="5"/>
+      <c r="AD29" s="5"/>
+      <c r="AE29" s="5"/>
+      <c r="AF29" s="24" t="s">
+        <v>258</v>
+      </c>
+      <c r="AH29" s="5"/>
+      <c r="AI29" s="5"/>
+      <c r="AJ29" s="5"/>
+      <c r="AK29" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL29" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM29" s="5">
+        <v>123</v>
+      </c>
+      <c r="AN29" s="7"/>
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>260</v>
+        <v>115</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="K30" t="s">
+        <v>45</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>278</v>
       </c>
       <c r="M30" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="T30" t="s">
-        <v>373</v>
-      </c>
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>268</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>47</v>
+        <v>260</v>
       </c>
       <c r="M31" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="T31" s="5"/>
+      <c r="T31" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="32" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>281</v>
@@ -6876,100 +6867,106 @@
       <c r="E32" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
+      <c r="F32" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="M32" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="R32" t="s">
-        <v>171</v>
-      </c>
-      <c r="S32" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y32" t="s">
-        <v>276</v>
-      </c>
-      <c r="Z32" t="s">
-        <v>342</v>
-      </c>
-      <c r="AB32" t="s">
-        <v>272</v>
-      </c>
-      <c r="AC32" s="25" t="s">
-        <v>273</v>
-      </c>
-      <c r="AD32" s="26">
-        <v>4</v>
-      </c>
-      <c r="AF32" s="25"/>
-      <c r="AG32" s="26"/>
+      <c r="T32" s="5"/>
     </row>
     <row r="33" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>230</v>
-      </c>
-      <c r="AE33" s="5" t="s">
-        <v>220</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="M33" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="R33" t="s">
+        <v>171</v>
+      </c>
+      <c r="S33" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>276</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>342</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>272</v>
+      </c>
+      <c r="AC33" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="AD33" s="26">
+        <v>4</v>
+      </c>
+      <c r="AF33" s="25"/>
+      <c r="AG33" s="26"/>
     </row>
     <row r="34" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>222</v>
-      </c>
-      <c r="AS34" t="s">
-        <v>388</v>
-      </c>
-      <c r="AT34" t="s">
-        <v>389</v>
+        <v>230</v>
+      </c>
+      <c r="AE34" s="5" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="35" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>224</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="D35" s="10"/>
-      <c r="O35" s="5"/>
-      <c r="R35" t="s">
-        <v>92</v>
-      </c>
-      <c r="S35" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC35" s="28" t="s">
-        <v>390</v>
-      </c>
-      <c r="AJ35" t="s">
-        <v>225</v>
+        <v>222</v>
+      </c>
+      <c r="AS35" t="s">
+        <v>388</v>
       </c>
       <c r="AT35" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="36" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>399</v>
-      </c>
-      <c r="C36" s="10"/>
+        <v>224</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>279</v>
+      </c>
       <c r="D36" s="10"/>
       <c r="O36" s="5"/>
-      <c r="AC36" s="28"/>
-      <c r="AE36" s="29" t="s">
-        <v>400</v>
-      </c>
-      <c r="AF36" t="s">
-        <v>398</v>
-      </c>
-      <c r="AI36" s="5" t="s">
-        <v>122</v>
+      <c r="R36" t="s">
+        <v>92</v>
+      </c>
+      <c r="S36" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC36" s="28" t="s">
+        <v>390</v>
+      </c>
+      <c r="AJ36" t="s">
+        <v>225</v>
+      </c>
+      <c r="AT36" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="37" spans="1:46" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>424</v>
+        <v>399</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
@@ -6982,35 +6979,36 @@
         <v>398</v>
       </c>
       <c r="AI37" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="38" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:46" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>403</v>
-      </c>
+        <v>424</v>
+      </c>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="O38" s="5"/>
+      <c r="AC38" s="28"/>
       <c r="AE38" s="29" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="AF38" t="s">
         <v>398</v>
       </c>
       <c r="AI38" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39" spans="1:46" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>478</v>
-      </c>
-      <c r="AE39" s="36" t="s">
-        <v>487</v>
+        <v>403</v>
+      </c>
+      <c r="AE39" s="29" t="s">
+        <v>397</v>
       </c>
       <c r="AF39" t="s">
-        <v>191</v>
-      </c>
-      <c r="AH39" s="36" t="s">
-        <v>487</v>
+        <v>398</v>
       </c>
       <c r="AI39" s="5" t="s">
         <v>122</v>
@@ -7018,61 +7016,64 @@
     </row>
     <row r="40" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>486</v>
-      </c>
-      <c r="AE40" s="37" t="s">
-        <v>485</v>
-      </c>
-      <c r="AI40" s="5"/>
+        <v>478</v>
+      </c>
+      <c r="AE40" s="36" t="s">
+        <v>487</v>
+      </c>
+      <c r="AF40" t="s">
+        <v>191</v>
+      </c>
+      <c r="AH40" s="36" t="s">
+        <v>487</v>
+      </c>
+      <c r="AI40" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="41" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>486</v>
+      </c>
+      <c r="AE41" s="37" t="s">
+        <v>485</v>
+      </c>
+      <c r="AI41" s="5"/>
+    </row>
+    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>477</v>
       </c>
-      <c r="AE41" s="36" t="s">
+      <c r="AE42" s="36" t="s">
         <v>387</v>
       </c>
-      <c r="AI41" s="5" t="s">
+      <c r="AI42" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:46" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="43" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>391</v>
       </c>
-      <c r="AE42" s="29" t="s">
+      <c r="AE43" s="29" t="s">
         <v>397</v>
       </c>
-      <c r="AF42" t="s">
+      <c r="AF43" t="s">
         <v>398</v>
       </c>
-      <c r="AI42" s="5" t="s">
+      <c r="AI43" s="5" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="43" spans="1:46" ht="60" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>414</v>
       </c>
-      <c r="AE43" s="29" t="s">
+      <c r="AE44" s="29" t="s">
         <v>415</v>
       </c>
-      <c r="AF43" s="34" t="s">
+      <c r="AF44" s="34" t="s">
         <v>416</v>
-      </c>
-      <c r="AI43" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="44" spans="1:46" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>419</v>
-      </c>
-      <c r="AE44" s="29" t="s">
-        <v>417</v>
-      </c>
-      <c r="AF44" s="34" t="s">
-        <v>418</v>
       </c>
       <c r="AI44" s="5" t="s">
         <v>122</v>
@@ -7080,7 +7081,7 @@
     </row>
     <row r="45" spans="1:46" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="AE45" s="29" t="s">
         <v>417</v>
@@ -7089,75 +7090,54 @@
         <v>418</v>
       </c>
       <c r="AI45" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="46" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:46" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AE46" s="29" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="AF46" s="34" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="AI46" s="5" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="47" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:46" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>428</v>
-      </c>
-      <c r="AE47" s="33" t="s">
-        <v>431</v>
+        <v>421</v>
+      </c>
+      <c r="AE47" s="29" t="s">
+        <v>415</v>
       </c>
       <c r="AF47" s="34" t="s">
-        <v>429</v>
+        <v>416</v>
       </c>
       <c r="AI47" s="5" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="48" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>392</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="R48" t="s">
-        <v>475</v>
-      </c>
-      <c r="S48" t="s">
-        <v>476</v>
-      </c>
-      <c r="T48" t="s">
-        <v>393</v>
-      </c>
-      <c r="U48" t="s">
-        <v>394</v>
-      </c>
-      <c r="V48" t="s">
-        <v>396</v>
-      </c>
-      <c r="W48" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="X48" s="5" t="s">
-        <v>93</v>
+        <v>428</v>
+      </c>
+      <c r="AE48" s="33" t="s">
+        <v>431</v>
+      </c>
+      <c r="AF48" s="34" t="s">
+        <v>429</v>
+      </c>
+      <c r="AI48" s="5" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="49" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>408</v>
+        <v>392</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>278</v>
@@ -7175,16 +7155,16 @@
         <v>476</v>
       </c>
       <c r="T49" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
       <c r="U49" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
       <c r="V49" t="s">
-        <v>404</v>
-      </c>
-      <c r="W49" s="31" t="s">
-        <v>407</v>
+        <v>396</v>
+      </c>
+      <c r="W49" s="5" t="s">
+        <v>395</v>
       </c>
       <c r="X49" s="5" t="s">
         <v>93</v>
@@ -7192,7 +7172,7 @@
     </row>
     <row r="50" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>278</v>
@@ -7209,76 +7189,76 @@
       <c r="S50" t="s">
         <v>476</v>
       </c>
-      <c r="T50" s="32" t="s">
-        <v>410</v>
-      </c>
-      <c r="U50" s="32" t="s">
-        <v>411</v>
-      </c>
-      <c r="V50" s="33" t="s">
-        <v>413</v>
+      <c r="T50" t="s">
+        <v>405</v>
+      </c>
+      <c r="U50" t="s">
+        <v>406</v>
+      </c>
+      <c r="V50" t="s">
+        <v>404</v>
       </c>
       <c r="W50" s="31" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="X50" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>401</v>
-      </c>
-      <c r="AO51" s="30" t="s">
-        <v>402</v>
+        <v>409</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="R51" t="s">
+        <v>475</v>
+      </c>
+      <c r="S51" t="s">
+        <v>476</v>
+      </c>
+      <c r="T51" s="32" t="s">
+        <v>410</v>
+      </c>
+      <c r="U51" s="32" t="s">
+        <v>411</v>
+      </c>
+      <c r="V51" s="33" t="s">
+        <v>413</v>
+      </c>
+      <c r="W51" s="31" t="s">
+        <v>412</v>
+      </c>
+      <c r="X51" s="5" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>401</v>
+      </c>
+      <c r="AO52" s="30" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="53" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>433</v>
       </c>
-      <c r="AO52" s="30" t="s">
+      <c r="AO53" s="30" t="s">
         <v>484</v>
-      </c>
-    </row>
-    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>422</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="R53" t="s">
-        <v>475</v>
-      </c>
-      <c r="S53" t="s">
-        <v>476</v>
-      </c>
-      <c r="T53" s="35" t="s">
-        <v>425</v>
-      </c>
-      <c r="U53" s="35" t="s">
-        <v>426</v>
-      </c>
-      <c r="V53" s="33" t="s">
-        <v>430</v>
-      </c>
-      <c r="W53" s="35" t="s">
-        <v>427</v>
-      </c>
-      <c r="X53" s="5" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="54" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>479</v>
+        <v>422</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>278</v>
@@ -7295,19 +7275,54 @@
       <c r="S54" t="s">
         <v>476</v>
       </c>
-      <c r="T54" t="s">
+      <c r="T54" s="35" t="s">
+        <v>425</v>
+      </c>
+      <c r="U54" s="35" t="s">
+        <v>426</v>
+      </c>
+      <c r="V54" s="33" t="s">
+        <v>430</v>
+      </c>
+      <c r="W54" s="35" t="s">
+        <v>427</v>
+      </c>
+      <c r="X54" s="5" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="55" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>479</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="R55" t="s">
+        <v>475</v>
+      </c>
+      <c r="S55" t="s">
+        <v>476</v>
+      </c>
+      <c r="T55" t="s">
         <v>480</v>
       </c>
-      <c r="U54" t="s">
+      <c r="U55" t="s">
         <v>481</v>
       </c>
-      <c r="V54" t="s">
+      <c r="V55" t="s">
         <v>482</v>
       </c>
-      <c r="W54" s="5" t="s">
+      <c r="W55" s="5" t="s">
         <v>483</v>
       </c>
-      <c r="X54" s="5" t="s">
+      <c r="X55" s="5" t="s">
         <v>93</v>
       </c>
     </row>
@@ -7317,44 +7332,44 @@
     <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-1600-000001000000}"/>
     <hyperlink ref="F2" r:id="rId3" display="Testers@278" xr:uid="{00000000-0004-0000-1600-000002000000}"/>
     <hyperlink ref="C2" r:id="rId4" display="lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{00000000-0004-0000-1600-000003000000}"/>
-    <hyperlink ref="E11" r:id="rId5" xr:uid="{00000000-0004-0000-1600-000004000000}"/>
-    <hyperlink ref="C12" r:id="rId6" xr:uid="{00000000-0004-0000-1600-000005000000}"/>
-    <hyperlink ref="C14" r:id="rId7" xr:uid="{00000000-0004-0000-1600-000006000000}"/>
-    <hyperlink ref="C15" r:id="rId8" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-1600-000007000000}"/>
-    <hyperlink ref="F15" r:id="rId9" xr:uid="{00000000-0004-0000-1600-000008000000}"/>
-    <hyperlink ref="B17" r:id="rId10" display="lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{00000000-0004-0000-1600-000009000000}"/>
-    <hyperlink ref="C17" r:id="rId11" display="lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{00000000-0004-0000-1600-00000A000000}"/>
-    <hyperlink ref="B18" r:id="rId12" xr:uid="{00000000-0004-0000-1600-00000B000000}"/>
-    <hyperlink ref="C18" r:id="rId13" xr:uid="{00000000-0004-0000-1600-00000C000000}"/>
-    <hyperlink ref="C28" r:id="rId14" xr:uid="{00000000-0004-0000-1600-00000D000000}"/>
+    <hyperlink ref="E12" r:id="rId5" xr:uid="{00000000-0004-0000-1600-000004000000}"/>
+    <hyperlink ref="C13" r:id="rId6" xr:uid="{00000000-0004-0000-1600-000005000000}"/>
+    <hyperlink ref="C15" r:id="rId7" xr:uid="{00000000-0004-0000-1600-000006000000}"/>
+    <hyperlink ref="C16" r:id="rId8" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-1600-000007000000}"/>
+    <hyperlink ref="F16" r:id="rId9" xr:uid="{00000000-0004-0000-1600-000008000000}"/>
+    <hyperlink ref="B18" r:id="rId10" display="lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{00000000-0004-0000-1600-000009000000}"/>
+    <hyperlink ref="C18" r:id="rId11" display="lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{00000000-0004-0000-1600-00000A000000}"/>
+    <hyperlink ref="B19" r:id="rId12" xr:uid="{00000000-0004-0000-1600-00000B000000}"/>
+    <hyperlink ref="C19" r:id="rId13" xr:uid="{00000000-0004-0000-1600-00000C000000}"/>
+    <hyperlink ref="C29" r:id="rId14" xr:uid="{00000000-0004-0000-1600-00000D000000}"/>
     <hyperlink ref="D2" r:id="rId15" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-1600-00000E000000}"/>
-    <hyperlink ref="L29" r:id="rId16" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-1600-00000F000000}"/>
-    <hyperlink ref="B31" r:id="rId17" xr:uid="{00000000-0004-0000-1600-000010000000}"/>
-    <hyperlink ref="C31" r:id="rId18" xr:uid="{00000000-0004-0000-1600-000011000000}"/>
-    <hyperlink ref="D31" r:id="rId19" xr:uid="{00000000-0004-0000-1600-000012000000}"/>
-    <hyperlink ref="E31" r:id="rId20" xr:uid="{00000000-0004-0000-1600-000013000000}"/>
-    <hyperlink ref="E32" r:id="rId21" xr:uid="{00000000-0004-0000-1600-000014000000}"/>
-    <hyperlink ref="B32" r:id="rId22" xr:uid="{00000000-0004-0000-1600-000015000000}"/>
-    <hyperlink ref="C32" r:id="rId23" xr:uid="{00000000-0004-0000-1600-000016000000}"/>
-    <hyperlink ref="D32" r:id="rId24" xr:uid="{00000000-0004-0000-1600-000017000000}"/>
-    <hyperlink ref="B11" r:id="rId25" xr:uid="{00000000-0004-0000-1600-000018000000}"/>
-    <hyperlink ref="B15" r:id="rId26" xr:uid="{00000000-0004-0000-1600-000019000000}"/>
-    <hyperlink ref="C35" r:id="rId27" xr:uid="{1864C442-0D98-42E4-A5FA-B81EFAA05600}"/>
-    <hyperlink ref="B48" r:id="rId28" display="testersemail.278@gmail.com" xr:uid="{34BD3CEC-6340-4CBD-96DC-8D004250BF84}"/>
-    <hyperlink ref="C48" r:id="rId29" display="testersemail.278@gmail.com" xr:uid="{F1625DAF-2FCD-401E-B451-0BDE8A534010}"/>
-    <hyperlink ref="D48" r:id="rId30" display="testersemail.278@gmail.com" xr:uid="{07702DCB-4B62-4824-BB8A-83439182C0EA}"/>
-    <hyperlink ref="B49" r:id="rId31" display="testersemail.278@gmail.com" xr:uid="{5B1965CC-AC91-4E74-81AB-F5894D8C2D9D}"/>
-    <hyperlink ref="C49" r:id="rId32" display="testersemail.278@gmail.com" xr:uid="{41C8C86C-6596-41A3-B56B-A8BC6862F5E2}"/>
-    <hyperlink ref="D49" r:id="rId33" display="testersemail.278@gmail.com" xr:uid="{6A001A27-2D56-448C-93B5-920CBED417DB}"/>
-    <hyperlink ref="B50" r:id="rId34" display="testersemail.278@gmail.com" xr:uid="{E91B6625-1005-4D68-8C77-C24DDB033C2B}"/>
-    <hyperlink ref="C50" r:id="rId35" display="testersemail.278@gmail.com" xr:uid="{015DE811-F050-4B71-96A8-193BA2EE4365}"/>
-    <hyperlink ref="D50" r:id="rId36" display="testersemail.278@gmail.com" xr:uid="{6A56F90F-8F22-4C03-B66D-47272E68A409}"/>
-    <hyperlink ref="B53" r:id="rId37" display="testersemail.278@gmail.com" xr:uid="{6ECC3E7A-0650-471A-8118-361B581591B2}"/>
-    <hyperlink ref="C53" r:id="rId38" display="testersemail.278@gmail.com" xr:uid="{FFDC6FD4-A6DF-4655-B604-131C2FEC8FCA}"/>
-    <hyperlink ref="D53" r:id="rId39" display="testersemail.278@gmail.com" xr:uid="{E68CD518-C7DB-4D2A-BFE5-92473B1B7D82}"/>
-    <hyperlink ref="B54" r:id="rId40" display="testersemail.278@gmail.com" xr:uid="{C068F1CE-D006-4174-81C1-E2703766A79B}"/>
-    <hyperlink ref="C54" r:id="rId41" display="testersemail.278@gmail.com" xr:uid="{2393F234-B92D-48CB-B748-088EB5B8D9F0}"/>
-    <hyperlink ref="D54" r:id="rId42" display="testersemail.278@gmail.com" xr:uid="{EB4696D1-B300-4BCB-8F2F-4D7BB5228026}"/>
+    <hyperlink ref="L30" r:id="rId16" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-1600-00000F000000}"/>
+    <hyperlink ref="B32" r:id="rId17" xr:uid="{00000000-0004-0000-1600-000010000000}"/>
+    <hyperlink ref="C32" r:id="rId18" xr:uid="{00000000-0004-0000-1600-000011000000}"/>
+    <hyperlink ref="D32" r:id="rId19" xr:uid="{00000000-0004-0000-1600-000012000000}"/>
+    <hyperlink ref="E32" r:id="rId20" xr:uid="{00000000-0004-0000-1600-000013000000}"/>
+    <hyperlink ref="E33" r:id="rId21" xr:uid="{00000000-0004-0000-1600-000014000000}"/>
+    <hyperlink ref="B33" r:id="rId22" xr:uid="{00000000-0004-0000-1600-000015000000}"/>
+    <hyperlink ref="C33" r:id="rId23" xr:uid="{00000000-0004-0000-1600-000016000000}"/>
+    <hyperlink ref="D33" r:id="rId24" xr:uid="{00000000-0004-0000-1600-000017000000}"/>
+    <hyperlink ref="B12" r:id="rId25" xr:uid="{00000000-0004-0000-1600-000018000000}"/>
+    <hyperlink ref="B16" r:id="rId26" xr:uid="{00000000-0004-0000-1600-000019000000}"/>
+    <hyperlink ref="C36" r:id="rId27" xr:uid="{1864C442-0D98-42E4-A5FA-B81EFAA05600}"/>
+    <hyperlink ref="B49" r:id="rId28" display="testersemail.278@gmail.com" xr:uid="{34BD3CEC-6340-4CBD-96DC-8D004250BF84}"/>
+    <hyperlink ref="C49" r:id="rId29" display="testersemail.278@gmail.com" xr:uid="{F1625DAF-2FCD-401E-B451-0BDE8A534010}"/>
+    <hyperlink ref="D49" r:id="rId30" display="testersemail.278@gmail.com" xr:uid="{07702DCB-4B62-4824-BB8A-83439182C0EA}"/>
+    <hyperlink ref="B50" r:id="rId31" display="testersemail.278@gmail.com" xr:uid="{5B1965CC-AC91-4E74-81AB-F5894D8C2D9D}"/>
+    <hyperlink ref="C50" r:id="rId32" display="testersemail.278@gmail.com" xr:uid="{41C8C86C-6596-41A3-B56B-A8BC6862F5E2}"/>
+    <hyperlink ref="D50" r:id="rId33" display="testersemail.278@gmail.com" xr:uid="{6A001A27-2D56-448C-93B5-920CBED417DB}"/>
+    <hyperlink ref="B51" r:id="rId34" display="testersemail.278@gmail.com" xr:uid="{E91B6625-1005-4D68-8C77-C24DDB033C2B}"/>
+    <hyperlink ref="C51" r:id="rId35" display="testersemail.278@gmail.com" xr:uid="{015DE811-F050-4B71-96A8-193BA2EE4365}"/>
+    <hyperlink ref="D51" r:id="rId36" display="testersemail.278@gmail.com" xr:uid="{6A56F90F-8F22-4C03-B66D-47272E68A409}"/>
+    <hyperlink ref="B54" r:id="rId37" display="testersemail.278@gmail.com" xr:uid="{6ECC3E7A-0650-471A-8118-361B581591B2}"/>
+    <hyperlink ref="C54" r:id="rId38" display="testersemail.278@gmail.com" xr:uid="{FFDC6FD4-A6DF-4655-B604-131C2FEC8FCA}"/>
+    <hyperlink ref="D54" r:id="rId39" display="testersemail.278@gmail.com" xr:uid="{E68CD518-C7DB-4D2A-BFE5-92473B1B7D82}"/>
+    <hyperlink ref="B55" r:id="rId40" display="testersemail.278@gmail.com" xr:uid="{C068F1CE-D006-4174-81C1-E2703766A79B}"/>
+    <hyperlink ref="C55" r:id="rId41" display="testersemail.278@gmail.com" xr:uid="{2393F234-B92D-48CB-B748-088EB5B8D9F0}"/>
+    <hyperlink ref="D55" r:id="rId42" display="testersemail.278@gmail.com" xr:uid="{EB4696D1-B300-4BCB-8F2F-4D7BB5228026}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId43"/>

</xml_diff>

<commit_message>
19 e2e testcase for osprey emea
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Osprey_EMEA/OSPEMEA_E2E_orderDetails.xlsx
+++ b/src/test/resources/TestData/Osprey_EMEA/OSPEMEA_E2E_orderDetails.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2B4251-673B-4526-8D09-30B66E679887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C412127E-5232-4261-85FD-534CDE4027BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="13" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1789" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1807" uniqueCount="497">
   <si>
     <t>UserName</t>
   </si>
@@ -1273,9 +1273,6 @@
     <t>Partial_Giftcard</t>
   </si>
   <si>
-    <t>4DU95D85Y5929Y53T88D</t>
-  </si>
-  <si>
     <t>SKU-10002926 -2QTY</t>
   </si>
   <si>
@@ -1535,6 +1532,30 @@
   </si>
   <si>
     <t>Standard Delivery (2-7 Days)</t>
+  </si>
+  <si>
+    <t>SKU-10004993 -2QTY IT</t>
+  </si>
+  <si>
+    <t>Sweden-IT Address</t>
+  </si>
+  <si>
+    <t>Via Biala 1</t>
+  </si>
+  <si>
+    <t>Laax Gr 2</t>
+  </si>
+  <si>
+    <t>Graubünden</t>
+  </si>
+  <si>
+    <t>7032</t>
+  </si>
+  <si>
+    <t>IT groundshipping</t>
+  </si>
+  <si>
+    <t>6YP53Z96N9485W79L66B</t>
   </si>
 </sst>
 </file>
@@ -2183,7 +2204,7 @@
         <v>15</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="AH1" s="1" t="s">
         <v>18</v>
@@ -2291,7 +2312,7 @@
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>278</v>
@@ -2323,16 +2344,16 @@
         <v>92</v>
       </c>
       <c r="U3" t="s">
+        <v>470</v>
+      </c>
+      <c r="V3" t="s">
+        <v>472</v>
+      </c>
+      <c r="W3" t="s">
         <v>471</v>
       </c>
-      <c r="V3" t="s">
+      <c r="X3" s="5" t="s">
         <v>473</v>
-      </c>
-      <c r="W3" t="s">
-        <v>472</v>
-      </c>
-      <c r="X3" s="5" t="s">
-        <v>474</v>
       </c>
       <c r="Y3" s="5" t="s">
         <v>93</v>
@@ -2346,16 +2367,16 @@
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>47</v>
@@ -2416,11 +2437,11 @@
         <v>204</v>
       </c>
       <c r="AF5" s="10" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="AG5" s="10"/>
       <c r="AH5" s="20" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AI5" s="9" t="s">
         <v>282</v>
@@ -2434,11 +2455,11 @@
     </row>
     <row r="6" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="N6" s="5"/>
       <c r="AF6" s="10" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="AG6" s="10"/>
       <c r="AH6" s="20"/>
@@ -2451,11 +2472,11 @@
     </row>
     <row r="7" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="N7" s="5"/>
       <c r="AF7" s="10" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="AG7" s="10"/>
       <c r="AH7" s="20"/>
@@ -2468,11 +2489,11 @@
     </row>
     <row r="8" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="N8" s="5"/>
       <c r="AF8" s="10" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="AG8" s="10"/>
       <c r="AH8" s="20"/>
@@ -2480,16 +2501,16 @@
         <v>282</v>
       </c>
       <c r="AK8" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="9" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="N9" s="5"/>
       <c r="AF9" s="10" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AG9" s="10"/>
       <c r="AH9" s="20"/>
@@ -2502,7 +2523,7 @@
     </row>
     <row r="10" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="N10" s="5"/>
       <c r="AF10" s="10" t="s">
@@ -2519,7 +2540,7 @@
     </row>
     <row r="11" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="N11" s="5"/>
       <c r="AF11" s="10" t="s">
@@ -2536,11 +2557,11 @@
     </row>
     <row r="12" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="N12" s="5"/>
       <c r="AF12" s="10" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="AG12" s="10"/>
       <c r="AH12" s="20"/>
@@ -2553,11 +2574,11 @@
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="N13" s="5"/>
       <c r="AF13" s="10" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="AG13" s="10"/>
       <c r="AH13" t="s">
@@ -2567,7 +2588,7 @@
         <v>282</v>
       </c>
       <c r="AJ13" s="10" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="AK13" s="5" t="s">
         <v>122</v>
@@ -2575,11 +2596,11 @@
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="N14" s="5"/>
       <c r="AF14" s="10" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="AG14" s="10"/>
       <c r="AH14" t="s">
@@ -2589,7 +2610,7 @@
         <v>282</v>
       </c>
       <c r="AJ14" s="10" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="AK14" s="5" t="s">
         <v>122</v>
@@ -2603,7 +2624,7 @@
         <v>204</v>
       </c>
       <c r="AL15" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.25">
@@ -2730,10 +2751,10 @@
         <v>44</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
@@ -2826,11 +2847,11 @@
         <v>141</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>204</v>
@@ -2891,16 +2912,16 @@
         <v>92</v>
       </c>
       <c r="U27" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="V27" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="W27" t="s">
         <v>316</v>
       </c>
       <c r="X27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="Y27" s="5" t="s">
         <v>93</v>
@@ -3043,10 +3064,10 @@
         <v>204</v>
       </c>
       <c r="AF30" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="AG30" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="AI30" s="5"/>
       <c r="AK30" s="5" t="s">
@@ -3061,7 +3082,7 @@
         <v>204</v>
       </c>
       <c r="AL31" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="32" spans="1:42" x14ac:dyDescent="0.25">
@@ -3123,7 +3144,7 @@
         <v>375</v>
       </c>
       <c r="P35" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="Q35" s="5" t="s">
         <v>207</v>
@@ -3137,7 +3158,7 @@
         <v>204</v>
       </c>
       <c r="AQ36" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="AR36" t="s">
         <v>242</v>
@@ -3239,7 +3260,7 @@
         <v>259</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="L40" t="s">
         <v>45</v>
@@ -3259,7 +3280,7 @@
         <v>204</v>
       </c>
       <c r="U41" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="42" spans="1:45" x14ac:dyDescent="0.25">
@@ -3267,19 +3288,19 @@
         <v>268</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="N42" s="5" t="s">
         <v>204</v>
@@ -3336,15 +3357,15 @@
         <v>283</v>
       </c>
       <c r="H44" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="45" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H45" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -5938,12 +5959,12 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
-  <dimension ref="A1:AT55"/>
+  <dimension ref="A1:AT58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6212,114 +6233,106 @@
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="M5" s="2"/>
       <c r="AJ5" s="5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>383</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="9"/>
-      <c r="M6" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="2"/>
-      <c r="Z6" s="5"/>
-      <c r="AA6" s="5"/>
-      <c r="AE6" s="5"/>
-      <c r="AF6" s="7"/>
-      <c r="AK6" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="AL6" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="AM6">
-        <v>123</v>
+        <v>495</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="AJ6" s="5" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>261</v>
-      </c>
-      <c r="M7" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="9"/>
+      <c r="M7" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="AJ7" t="s">
-        <v>262</v>
+      <c r="N7" s="2"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="2"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="7"/>
+      <c r="AK7" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="AL7" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM7">
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>99</v>
-      </c>
-      <c r="M8" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="AK8" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="AL8" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="AM8">
-        <v>123</v>
+      <c r="AJ8" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>102</v>
-      </c>
-      <c r="M9" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M9" s="5" t="s">
         <v>204</v>
       </c>
       <c r="AK9" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="AL9" s="7" t="s">
         <v>101</v>
       </c>
       <c r="AM9">
-        <v>1234</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>104</v>
-      </c>
-      <c r="M10" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="M10" s="2" t="s">
         <v>204</v>
       </c>
       <c r="AK10" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="AL10" s="7" t="s">
         <v>101</v>
       </c>
       <c r="AM10">
-        <v>123</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>106</v>
-      </c>
-      <c r="M11" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M11" s="5" t="s">
         <v>204</v>
       </c>
       <c r="AK11" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AL11" s="7" t="s">
         <v>101</v>
@@ -6330,214 +6343,173 @@
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="M12" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" t="s">
-        <v>45</v>
-      </c>
-      <c r="S12" t="s">
-        <v>46</v>
+      <c r="AK12" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL12" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM12">
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>111</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>74</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="M13" s="2" t="s">
+      <c r="E13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="5" t="s">
         <v>204</v>
       </c>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
       <c r="R13" t="s">
         <v>45</v>
       </c>
       <c r="S13" t="s">
-        <v>73</v>
-      </c>
-      <c r="T13" s="2"/>
-      <c r="U13" t="s">
-        <v>176</v>
-      </c>
-      <c r="V13" t="s">
-        <v>175</v>
-      </c>
-      <c r="W13" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="X13" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y13" s="5"/>
-      <c r="Z13" s="5"/>
-      <c r="AA13" s="5"/>
-      <c r="AB13" s="5"/>
-      <c r="AC13" s="5"/>
-      <c r="AD13" s="5"/>
-      <c r="AF13" s="5"/>
-      <c r="AG13" s="5"/>
-      <c r="AH13" s="5"/>
-      <c r="AI13" s="5"/>
+        <v>46</v>
+      </c>
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>112</v>
-      </c>
-      <c r="M14" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="M14" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="AK14" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="AL14" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="AM14">
-        <v>12</v>
-      </c>
+      <c r="R14" t="s">
+        <v>45</v>
+      </c>
+      <c r="S14" t="s">
+        <v>73</v>
+      </c>
+      <c r="T14" s="2"/>
+      <c r="U14" t="s">
+        <v>176</v>
+      </c>
+      <c r="V14" t="s">
+        <v>175</v>
+      </c>
+      <c r="W14" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="X14" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="5"/>
+      <c r="AF14" s="5"/>
+      <c r="AG14" s="5"/>
+      <c r="AH14" s="5"/>
+      <c r="AI14" s="5"/>
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>141</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="M15" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="M15" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="AF15" s="5"/>
-      <c r="AG15" s="5"/>
+      <c r="AK15" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="AL15" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="AM15">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>144</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>294</v>
+        <v>141</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>278</v>
+        <v>143</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="5" t="s">
+      <c r="E16" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="M16" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="AF16" s="5"/>
+      <c r="AG16" s="5"/>
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>146</v>
-      </c>
-      <c r="M17" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="R17" t="s">
-        <v>46</v>
-      </c>
-      <c r="S17" t="s">
-        <v>92</v>
-      </c>
-      <c r="T17" t="s">
-        <v>243</v>
-      </c>
-      <c r="U17" t="s">
-        <v>244</v>
-      </c>
-      <c r="V17" t="s">
-        <v>245</v>
-      </c>
-      <c r="W17" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="X17" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y17" s="5"/>
-      <c r="Z17" s="5"/>
-      <c r="AA17" s="5"/>
-      <c r="AB17" s="5"/>
-      <c r="AC17" s="5"/>
-      <c r="AD17" s="5"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>151</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="M18" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
       <c r="R18" t="s">
         <v>46</v>
       </c>
@@ -6545,16 +6517,16 @@
         <v>92</v>
       </c>
       <c r="T18" t="s">
-        <v>152</v>
+        <v>243</v>
       </c>
       <c r="U18" t="s">
-        <v>153</v>
+        <v>244</v>
       </c>
       <c r="V18" t="s">
-        <v>154</v>
+        <v>245</v>
       </c>
       <c r="W18" s="5" t="s">
-        <v>155</v>
+        <v>246</v>
       </c>
       <c r="X18" s="5" t="s">
         <v>93</v>
@@ -6565,21 +6537,18 @@
       <c r="AB18" s="5"/>
       <c r="AC18" s="5"/>
       <c r="AD18" s="5"/>
-      <c r="AG18" s="5"/>
-      <c r="AI18" s="5"/>
-      <c r="AJ18" s="7"/>
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>156</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="D19" s="10"/>
+        <v>151</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="9" t="s">
         <v>47</v>
       </c>
@@ -6592,7 +6561,7 @@
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
-      <c r="M19" s="2" t="s">
+      <c r="M19" s="5" t="s">
         <v>204</v>
       </c>
       <c r="N19" s="9"/>
@@ -6606,16 +6575,16 @@
         <v>92</v>
       </c>
       <c r="T19" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="U19" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="V19" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="W19" s="5" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="X19" s="5" t="s">
         <v>93</v>
@@ -6626,130 +6595,180 @@
       <c r="AB19" s="5"/>
       <c r="AC19" s="5"/>
       <c r="AD19" s="5"/>
-      <c r="AE19" s="5"/>
+      <c r="AG19" s="5"/>
+      <c r="AI19" s="5"/>
+      <c r="AJ19" s="7"/>
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>166</v>
-      </c>
-      <c r="M20" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="AE20" t="s">
-        <v>263</v>
-      </c>
-      <c r="AG20" s="5"/>
-      <c r="AI20" s="5" t="s">
-        <v>72</v>
-      </c>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" t="s">
+        <v>46</v>
+      </c>
+      <c r="S20" t="s">
+        <v>92</v>
+      </c>
+      <c r="T20" t="s">
+        <v>158</v>
+      </c>
+      <c r="U20" t="s">
+        <v>159</v>
+      </c>
+      <c r="V20" t="s">
+        <v>160</v>
+      </c>
+      <c r="W20" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="X20" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y20" s="5"/>
+      <c r="Z20" s="5"/>
+      <c r="AA20" s="5"/>
+      <c r="AB20" s="5"/>
+      <c r="AC20" s="5"/>
+      <c r="AD20" s="5"/>
+      <c r="AE20" s="5"/>
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>178</v>
-      </c>
-      <c r="M21" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="M21" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="AJ21" s="5" t="s">
-        <v>299</v>
+      <c r="AE21" t="s">
+        <v>263</v>
+      </c>
+      <c r="AG21" s="5"/>
+      <c r="AI21" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>186</v>
-      </c>
-      <c r="M22" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="M22" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="N22" t="s">
-        <v>208</v>
-      </c>
-      <c r="R22" t="s">
-        <v>46</v>
-      </c>
-      <c r="S22" t="s">
-        <v>92</v>
-      </c>
-      <c r="AN22" t="s">
-        <v>187</v>
+      <c r="AJ22" s="5" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>91</v>
-      </c>
-      <c r="M23" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="M23" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="AI23" s="5" t="s">
-        <v>72</v>
+      <c r="N23" t="s">
+        <v>208</v>
+      </c>
+      <c r="R23" t="s">
+        <v>46</v>
+      </c>
+      <c r="S23" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN23" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>201</v>
-      </c>
-      <c r="G24" t="s">
-        <v>201</v>
-      </c>
-      <c r="H24" t="s">
-        <v>264</v>
-      </c>
-      <c r="M24" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="M24" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="Q24" t="s">
-        <v>265</v>
+      <c r="AI24" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="G25" t="s">
+        <v>201</v>
+      </c>
+      <c r="H25" t="s">
+        <v>264</v>
       </c>
       <c r="M25" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="N25" t="s">
-        <v>375</v>
-      </c>
-      <c r="O25" s="5" t="s">
-        <v>350</v>
-      </c>
-      <c r="P25" s="5" t="s">
-        <v>207</v>
+      <c r="Q25" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>230</v>
+        <v>203</v>
       </c>
       <c r="M26" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="AO26" t="s">
-        <v>242</v>
-      </c>
-      <c r="AP26" t="s">
-        <v>242</v>
-      </c>
-      <c r="AQ26" t="s">
-        <v>229</v>
+      <c r="N26" t="s">
+        <v>375</v>
+      </c>
+      <c r="O26" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="P26" s="5" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>253</v>
+        <v>230</v>
       </c>
       <c r="M27" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="AE27" t="s">
-        <v>252</v>
+      <c r="AO27" t="s">
+        <v>242</v>
+      </c>
+      <c r="AP27" t="s">
+        <v>242</v>
+      </c>
+      <c r="AQ27" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="M28" s="5" t="s">
         <v>204</v>
@@ -6760,124 +6779,111 @@
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>256</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D29" s="10"/>
+        <v>255</v>
+      </c>
       <c r="M29" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
-      <c r="R29" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="S29" t="s">
-        <v>45</v>
-      </c>
-      <c r="T29" t="s">
-        <v>243</v>
-      </c>
-      <c r="U29" t="s">
-        <v>244</v>
-      </c>
-      <c r="V29" t="s">
-        <v>245</v>
-      </c>
-      <c r="W29" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="X29" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="Y29" s="5"/>
-      <c r="Z29" s="5"/>
-      <c r="AA29" s="5">
-        <v>888888</v>
-      </c>
-      <c r="AB29" s="5"/>
-      <c r="AC29" s="5"/>
-      <c r="AD29" s="5"/>
-      <c r="AE29" s="5"/>
-      <c r="AF29" s="24" t="s">
-        <v>258</v>
-      </c>
-      <c r="AH29" s="5"/>
-      <c r="AI29" s="5"/>
-      <c r="AJ29" s="5"/>
-      <c r="AK29" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="AL29" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="AM29" s="5">
-        <v>123</v>
-      </c>
-      <c r="AN29" s="7"/>
+      <c r="AE29" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>115</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="K30" t="s">
-        <v>45</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>278</v>
-      </c>
+        <v>256</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="10"/>
       <c r="M30" s="5" t="s">
         <v>204</v>
       </c>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="S30" t="s">
+        <v>45</v>
+      </c>
+      <c r="T30" t="s">
+        <v>243</v>
+      </c>
+      <c r="U30" t="s">
+        <v>244</v>
+      </c>
+      <c r="V30" t="s">
+        <v>245</v>
+      </c>
+      <c r="W30" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="X30" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="Y30" s="5"/>
+      <c r="Z30" s="5"/>
+      <c r="AA30" s="5">
+        <v>888888</v>
+      </c>
+      <c r="AB30" s="5"/>
+      <c r="AC30" s="5"/>
+      <c r="AD30" s="5"/>
+      <c r="AE30" s="5"/>
+      <c r="AF30" s="24" t="s">
+        <v>258</v>
+      </c>
+      <c r="AH30" s="5"/>
+      <c r="AI30" s="5"/>
+      <c r="AJ30" s="5"/>
+      <c r="AK30" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL30" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM30" s="5">
+        <v>123</v>
+      </c>
+      <c r="AN30" s="7"/>
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>260</v>
+        <v>115</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="K31" t="s">
+        <v>45</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>278</v>
       </c>
       <c r="M31" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="T31" t="s">
-        <v>373</v>
-      </c>
     </row>
     <row r="32" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>268</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>47</v>
+        <v>260</v>
       </c>
       <c r="M32" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="T32" s="5"/>
+      <c r="T32" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="33" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>281</v>
@@ -6891,100 +6897,106 @@
       <c r="E33" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
+      <c r="F33" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="M33" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="R33" t="s">
-        <v>171</v>
-      </c>
-      <c r="S33" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y33" t="s">
-        <v>276</v>
-      </c>
-      <c r="Z33" t="s">
-        <v>342</v>
-      </c>
-      <c r="AB33" t="s">
-        <v>272</v>
-      </c>
-      <c r="AC33" s="25" t="s">
-        <v>273</v>
-      </c>
-      <c r="AD33" s="26">
-        <v>4</v>
-      </c>
-      <c r="AF33" s="25"/>
-      <c r="AG33" s="26"/>
+      <c r="T33" s="5"/>
     </row>
     <row r="34" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>230</v>
-      </c>
-      <c r="AE34" s="5" t="s">
-        <v>220</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="M34" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="R34" t="s">
+        <v>171</v>
+      </c>
+      <c r="S34" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>276</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>342</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>272</v>
+      </c>
+      <c r="AC34" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="AD34" s="26">
+        <v>4</v>
+      </c>
+      <c r="AF34" s="25"/>
+      <c r="AG34" s="26"/>
     </row>
     <row r="35" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>222</v>
-      </c>
-      <c r="AS35" t="s">
-        <v>388</v>
-      </c>
-      <c r="AT35" t="s">
-        <v>389</v>
+        <v>230</v>
+      </c>
+      <c r="AE35" s="5" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="36" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>224</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="D36" s="10"/>
-      <c r="O36" s="5"/>
-      <c r="R36" t="s">
-        <v>92</v>
-      </c>
-      <c r="S36" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC36" s="28" t="s">
-        <v>390</v>
-      </c>
-      <c r="AJ36" t="s">
-        <v>225</v>
+        <v>222</v>
+      </c>
+      <c r="AS36" t="s">
+        <v>388</v>
       </c>
       <c r="AT36" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="37" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>399</v>
-      </c>
-      <c r="C37" s="10"/>
+        <v>224</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>279</v>
+      </c>
       <c r="D37" s="10"/>
       <c r="O37" s="5"/>
-      <c r="AC37" s="28"/>
-      <c r="AE37" s="29" t="s">
-        <v>400</v>
-      </c>
-      <c r="AF37" t="s">
-        <v>398</v>
-      </c>
-      <c r="AI37" s="5" t="s">
-        <v>122</v>
+      <c r="R37" t="s">
+        <v>92</v>
+      </c>
+      <c r="S37" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC37" s="28" t="s">
+        <v>390</v>
+      </c>
+      <c r="AJ37" t="s">
+        <v>225</v>
+      </c>
+      <c r="AT37" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="38" spans="1:46" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>424</v>
+        <v>399</v>
       </c>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
@@ -6997,83 +7009,94 @@
         <v>398</v>
       </c>
       <c r="AI38" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:46" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>489</v>
+      </c>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="O39" s="5"/>
+      <c r="AC39" s="28"/>
+      <c r="AE39" s="36" t="s">
+        <v>400</v>
+      </c>
+      <c r="AF39" t="s">
+        <v>191</v>
+      </c>
+      <c r="AH39" s="36" t="s">
+        <v>400</v>
+      </c>
+      <c r="AI39" s="37" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>423</v>
+      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="O40" s="5"/>
+      <c r="AC40" s="28"/>
+      <c r="AE40" s="29" t="s">
+        <v>400</v>
+      </c>
+      <c r="AF40" t="s">
+        <v>398</v>
+      </c>
+      <c r="AI40" s="5" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="39" spans="1:46" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>403</v>
-      </c>
-      <c r="AE39" s="29" t="s">
+    <row r="41" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>402</v>
+      </c>
+      <c r="AE41" s="29" t="s">
         <v>397</v>
       </c>
-      <c r="AF39" t="s">
+      <c r="AF41" t="s">
         <v>398</v>
       </c>
-      <c r="AI39" s="5" t="s">
+      <c r="AI41" s="5" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>478</v>
-      </c>
-      <c r="AE40" s="36" t="s">
-        <v>487</v>
-      </c>
-      <c r="AF40" t="s">
-        <v>191</v>
-      </c>
-      <c r="AH40" s="36" t="s">
-        <v>487</v>
-      </c>
-      <c r="AI40" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>486</v>
-      </c>
-      <c r="AE41" s="37" t="s">
-        <v>485</v>
-      </c>
-      <c r="AI41" s="5"/>
     </row>
     <row r="42" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>477</v>
       </c>
       <c r="AE42" s="36" t="s">
-        <v>387</v>
+        <v>486</v>
+      </c>
+      <c r="AF42" t="s">
+        <v>191</v>
+      </c>
+      <c r="AH42" s="36" t="s">
+        <v>486</v>
       </c>
       <c r="AI42" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>391</v>
-      </c>
-      <c r="AE43" s="29" t="s">
-        <v>397</v>
-      </c>
-      <c r="AF43" t="s">
-        <v>398</v>
-      </c>
-      <c r="AI43" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="44" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+        <v>485</v>
+      </c>
+      <c r="AE43" s="37" t="s">
+        <v>484</v>
+      </c>
+      <c r="AI43" s="5"/>
+    </row>
+    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>414</v>
-      </c>
-      <c r="AE44" s="29" t="s">
-        <v>415</v>
-      </c>
-      <c r="AF44" s="34" t="s">
-        <v>416</v>
+        <v>476</v>
+      </c>
+      <c r="AE44" s="36" t="s">
+        <v>387</v>
       </c>
       <c r="AI44" s="5" t="s">
         <v>122</v>
@@ -7081,133 +7104,91 @@
     </row>
     <row r="45" spans="1:46" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>391</v>
+      </c>
+      <c r="AE45" s="29" t="s">
+        <v>397</v>
+      </c>
+      <c r="AF45" t="s">
+        <v>398</v>
+      </c>
+      <c r="AI45" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="46" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>413</v>
+      </c>
+      <c r="AE46" s="29" t="s">
+        <v>414</v>
+      </c>
+      <c r="AF46" s="34" t="s">
+        <v>415</v>
+      </c>
+      <c r="AI46" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>418</v>
+      </c>
+      <c r="AE47" s="29" t="s">
+        <v>416</v>
+      </c>
+      <c r="AF47" s="34" t="s">
+        <v>417</v>
+      </c>
+      <c r="AI47" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>419</v>
       </c>
-      <c r="AE45" s="29" t="s">
+      <c r="AE48" s="29" t="s">
+        <v>416</v>
+      </c>
+      <c r="AF48" s="34" t="s">
         <v>417</v>
-      </c>
-      <c r="AF45" s="34" t="s">
-        <v>418</v>
-      </c>
-      <c r="AI45" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="46" spans="1:46" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>420</v>
-      </c>
-      <c r="AE46" s="29" t="s">
-        <v>417</v>
-      </c>
-      <c r="AF46" s="34" t="s">
-        <v>418</v>
-      </c>
-      <c r="AI46" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="47" spans="1:46" ht="60" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>421</v>
-      </c>
-      <c r="AE47" s="29" t="s">
-        <v>415</v>
-      </c>
-      <c r="AF47" s="34" t="s">
-        <v>416</v>
-      </c>
-      <c r="AI47" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="48" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>428</v>
-      </c>
-      <c r="AE48" s="33" t="s">
-        <v>431</v>
-      </c>
-      <c r="AF48" s="34" t="s">
-        <v>429</v>
       </c>
       <c r="AI48" s="5" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="49" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:41" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>392</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="R49" t="s">
-        <v>475</v>
-      </c>
-      <c r="S49" t="s">
-        <v>476</v>
-      </c>
-      <c r="T49" t="s">
-        <v>393</v>
-      </c>
-      <c r="U49" t="s">
-        <v>394</v>
-      </c>
-      <c r="V49" t="s">
-        <v>396</v>
-      </c>
-      <c r="W49" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="X49" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="50" spans="1:41" x14ac:dyDescent="0.25">
+        <v>420</v>
+      </c>
+      <c r="AE49" s="29" t="s">
+        <v>414</v>
+      </c>
+      <c r="AF49" s="34" t="s">
+        <v>415</v>
+      </c>
+      <c r="AI49" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="50" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>408</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="R50" t="s">
-        <v>475</v>
-      </c>
-      <c r="S50" t="s">
-        <v>476</v>
-      </c>
-      <c r="T50" t="s">
-        <v>405</v>
-      </c>
-      <c r="U50" t="s">
-        <v>406</v>
-      </c>
-      <c r="V50" t="s">
-        <v>404</v>
-      </c>
-      <c r="W50" s="31" t="s">
-        <v>407</v>
-      </c>
-      <c r="X50" s="5" t="s">
-        <v>93</v>
+        <v>427</v>
+      </c>
+      <c r="AE50" s="33" t="s">
+        <v>430</v>
+      </c>
+      <c r="AF50" s="34" t="s">
+        <v>428</v>
+      </c>
+      <c r="AI50" s="5" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="51" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>409</v>
+        <v>392</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>278</v>
@@ -7219,110 +7200,215 @@
         <v>278</v>
       </c>
       <c r="R51" t="s">
+        <v>474</v>
+      </c>
+      <c r="S51" t="s">
         <v>475</v>
       </c>
-      <c r="S51" t="s">
-        <v>476</v>
-      </c>
-      <c r="T51" s="32" t="s">
-        <v>410</v>
-      </c>
-      <c r="U51" s="32" t="s">
-        <v>411</v>
-      </c>
-      <c r="V51" s="33" t="s">
-        <v>413</v>
-      </c>
-      <c r="W51" s="31" t="s">
-        <v>412</v>
+      <c r="T51" t="s">
+        <v>393</v>
+      </c>
+      <c r="U51" t="s">
+        <v>394</v>
+      </c>
+      <c r="V51" t="s">
+        <v>396</v>
+      </c>
+      <c r="W51" s="5" t="s">
+        <v>395</v>
       </c>
       <c r="X51" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="52" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>407</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="R52" t="s">
+        <v>474</v>
+      </c>
+      <c r="S52" t="s">
+        <v>475</v>
+      </c>
+      <c r="T52" t="s">
+        <v>404</v>
+      </c>
+      <c r="U52" t="s">
+        <v>405</v>
+      </c>
+      <c r="V52" t="s">
+        <v>403</v>
+      </c>
+      <c r="W52" s="31" t="s">
+        <v>406</v>
+      </c>
+      <c r="X52" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>408</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="R53" t="s">
+        <v>474</v>
+      </c>
+      <c r="S53" t="s">
+        <v>475</v>
+      </c>
+      <c r="T53" s="32" t="s">
+        <v>409</v>
+      </c>
+      <c r="U53" s="32" t="s">
+        <v>410</v>
+      </c>
+      <c r="V53" s="33" t="s">
+        <v>412</v>
+      </c>
+      <c r="W53" s="31" t="s">
+        <v>411</v>
+      </c>
+      <c r="X53" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>401</v>
       </c>
-      <c r="AO52" s="30" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="53" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>433</v>
-      </c>
-      <c r="AO53" s="30" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="54" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="AO54" s="30" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="55" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>432</v>
+      </c>
+      <c r="AO55" s="30" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="56" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>421</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="R56" t="s">
+        <v>474</v>
+      </c>
+      <c r="S56" t="s">
+        <v>475</v>
+      </c>
+      <c r="T56" s="35" t="s">
+        <v>424</v>
+      </c>
+      <c r="U56" s="35" t="s">
+        <v>425</v>
+      </c>
+      <c r="V56" s="33" t="s">
+        <v>429</v>
+      </c>
+      <c r="W56" s="35" t="s">
+        <v>426</v>
+      </c>
+      <c r="X56" s="5" t="s">
         <v>422</v>
       </c>
-      <c r="B54" s="2" t="s">
+    </row>
+    <row r="57" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>478</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="R54" t="s">
+      <c r="R57" t="s">
+        <v>474</v>
+      </c>
+      <c r="S57" t="s">
         <v>475</v>
       </c>
-      <c r="S54" t="s">
-        <v>476</v>
-      </c>
-      <c r="T54" s="35" t="s">
-        <v>425</v>
-      </c>
-      <c r="U54" s="35" t="s">
-        <v>426</v>
-      </c>
-      <c r="V54" s="33" t="s">
-        <v>430</v>
-      </c>
-      <c r="W54" s="35" t="s">
-        <v>427</v>
-      </c>
-      <c r="X54" s="5" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="55" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="T57" t="s">
         <v>479</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="U57" t="s">
+        <v>480</v>
+      </c>
+      <c r="V57" t="s">
+        <v>481</v>
+      </c>
+      <c r="W57" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="X57" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>490</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="R55" t="s">
+      <c r="R58" t="s">
+        <v>474</v>
+      </c>
+      <c r="S58" t="s">
         <v>475</v>
       </c>
-      <c r="S55" t="s">
-        <v>476</v>
-      </c>
-      <c r="T55" t="s">
-        <v>480</v>
-      </c>
-      <c r="U55" t="s">
-        <v>481</v>
-      </c>
-      <c r="V55" t="s">
-        <v>482</v>
-      </c>
-      <c r="W55" s="5" t="s">
-        <v>483</v>
-      </c>
-      <c r="X55" s="5" t="s">
+      <c r="T58" t="s">
+        <v>491</v>
+      </c>
+      <c r="U58" t="s">
+        <v>492</v>
+      </c>
+      <c r="V58" t="s">
+        <v>493</v>
+      </c>
+      <c r="W58" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="X58" s="5" t="s">
         <v>93</v>
       </c>
     </row>
@@ -7332,47 +7418,50 @@
     <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-1600-000001000000}"/>
     <hyperlink ref="F2" r:id="rId3" display="Testers@278" xr:uid="{00000000-0004-0000-1600-000002000000}"/>
     <hyperlink ref="C2" r:id="rId4" display="lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{00000000-0004-0000-1600-000003000000}"/>
-    <hyperlink ref="E12" r:id="rId5" xr:uid="{00000000-0004-0000-1600-000004000000}"/>
-    <hyperlink ref="C13" r:id="rId6" xr:uid="{00000000-0004-0000-1600-000005000000}"/>
-    <hyperlink ref="C15" r:id="rId7" xr:uid="{00000000-0004-0000-1600-000006000000}"/>
-    <hyperlink ref="C16" r:id="rId8" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-1600-000007000000}"/>
-    <hyperlink ref="F16" r:id="rId9" xr:uid="{00000000-0004-0000-1600-000008000000}"/>
-    <hyperlink ref="B18" r:id="rId10" display="lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{00000000-0004-0000-1600-000009000000}"/>
-    <hyperlink ref="C18" r:id="rId11" display="lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{00000000-0004-0000-1600-00000A000000}"/>
-    <hyperlink ref="B19" r:id="rId12" xr:uid="{00000000-0004-0000-1600-00000B000000}"/>
-    <hyperlink ref="C19" r:id="rId13" xr:uid="{00000000-0004-0000-1600-00000C000000}"/>
-    <hyperlink ref="C29" r:id="rId14" xr:uid="{00000000-0004-0000-1600-00000D000000}"/>
+    <hyperlink ref="E13" r:id="rId5" xr:uid="{00000000-0004-0000-1600-000004000000}"/>
+    <hyperlink ref="C14" r:id="rId6" xr:uid="{00000000-0004-0000-1600-000005000000}"/>
+    <hyperlink ref="C16" r:id="rId7" xr:uid="{00000000-0004-0000-1600-000006000000}"/>
+    <hyperlink ref="C17" r:id="rId8" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-1600-000007000000}"/>
+    <hyperlink ref="F17" r:id="rId9" xr:uid="{00000000-0004-0000-1600-000008000000}"/>
+    <hyperlink ref="B19" r:id="rId10" display="lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{00000000-0004-0000-1600-000009000000}"/>
+    <hyperlink ref="C19" r:id="rId11" display="lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{00000000-0004-0000-1600-00000A000000}"/>
+    <hyperlink ref="B20" r:id="rId12" xr:uid="{00000000-0004-0000-1600-00000B000000}"/>
+    <hyperlink ref="C20" r:id="rId13" xr:uid="{00000000-0004-0000-1600-00000C000000}"/>
+    <hyperlink ref="C30" r:id="rId14" xr:uid="{00000000-0004-0000-1600-00000D000000}"/>
     <hyperlink ref="D2" r:id="rId15" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-1600-00000E000000}"/>
-    <hyperlink ref="L30" r:id="rId16" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-1600-00000F000000}"/>
-    <hyperlink ref="B32" r:id="rId17" xr:uid="{00000000-0004-0000-1600-000010000000}"/>
-    <hyperlink ref="C32" r:id="rId18" xr:uid="{00000000-0004-0000-1600-000011000000}"/>
-    <hyperlink ref="D32" r:id="rId19" xr:uid="{00000000-0004-0000-1600-000012000000}"/>
-    <hyperlink ref="E32" r:id="rId20" xr:uid="{00000000-0004-0000-1600-000013000000}"/>
-    <hyperlink ref="E33" r:id="rId21" xr:uid="{00000000-0004-0000-1600-000014000000}"/>
-    <hyperlink ref="B33" r:id="rId22" xr:uid="{00000000-0004-0000-1600-000015000000}"/>
-    <hyperlink ref="C33" r:id="rId23" xr:uid="{00000000-0004-0000-1600-000016000000}"/>
-    <hyperlink ref="D33" r:id="rId24" xr:uid="{00000000-0004-0000-1600-000017000000}"/>
-    <hyperlink ref="B12" r:id="rId25" xr:uid="{00000000-0004-0000-1600-000018000000}"/>
-    <hyperlink ref="B16" r:id="rId26" xr:uid="{00000000-0004-0000-1600-000019000000}"/>
-    <hyperlink ref="C36" r:id="rId27" xr:uid="{1864C442-0D98-42E4-A5FA-B81EFAA05600}"/>
-    <hyperlink ref="B49" r:id="rId28" display="testersemail.278@gmail.com" xr:uid="{34BD3CEC-6340-4CBD-96DC-8D004250BF84}"/>
-    <hyperlink ref="C49" r:id="rId29" display="testersemail.278@gmail.com" xr:uid="{F1625DAF-2FCD-401E-B451-0BDE8A534010}"/>
-    <hyperlink ref="D49" r:id="rId30" display="testersemail.278@gmail.com" xr:uid="{07702DCB-4B62-4824-BB8A-83439182C0EA}"/>
-    <hyperlink ref="B50" r:id="rId31" display="testersemail.278@gmail.com" xr:uid="{5B1965CC-AC91-4E74-81AB-F5894D8C2D9D}"/>
-    <hyperlink ref="C50" r:id="rId32" display="testersemail.278@gmail.com" xr:uid="{41C8C86C-6596-41A3-B56B-A8BC6862F5E2}"/>
-    <hyperlink ref="D50" r:id="rId33" display="testersemail.278@gmail.com" xr:uid="{6A001A27-2D56-448C-93B5-920CBED417DB}"/>
-    <hyperlink ref="B51" r:id="rId34" display="testersemail.278@gmail.com" xr:uid="{E91B6625-1005-4D68-8C77-C24DDB033C2B}"/>
-    <hyperlink ref="C51" r:id="rId35" display="testersemail.278@gmail.com" xr:uid="{015DE811-F050-4B71-96A8-193BA2EE4365}"/>
-    <hyperlink ref="D51" r:id="rId36" display="testersemail.278@gmail.com" xr:uid="{6A56F90F-8F22-4C03-B66D-47272E68A409}"/>
-    <hyperlink ref="B54" r:id="rId37" display="testersemail.278@gmail.com" xr:uid="{6ECC3E7A-0650-471A-8118-361B581591B2}"/>
-    <hyperlink ref="C54" r:id="rId38" display="testersemail.278@gmail.com" xr:uid="{FFDC6FD4-A6DF-4655-B604-131C2FEC8FCA}"/>
-    <hyperlink ref="D54" r:id="rId39" display="testersemail.278@gmail.com" xr:uid="{E68CD518-C7DB-4D2A-BFE5-92473B1B7D82}"/>
-    <hyperlink ref="B55" r:id="rId40" display="testersemail.278@gmail.com" xr:uid="{C068F1CE-D006-4174-81C1-E2703766A79B}"/>
-    <hyperlink ref="C55" r:id="rId41" display="testersemail.278@gmail.com" xr:uid="{2393F234-B92D-48CB-B748-088EB5B8D9F0}"/>
-    <hyperlink ref="D55" r:id="rId42" display="testersemail.278@gmail.com" xr:uid="{EB4696D1-B300-4BCB-8F2F-4D7BB5228026}"/>
+    <hyperlink ref="L31" r:id="rId16" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-1600-00000F000000}"/>
+    <hyperlink ref="B33" r:id="rId17" xr:uid="{00000000-0004-0000-1600-000010000000}"/>
+    <hyperlink ref="C33" r:id="rId18" xr:uid="{00000000-0004-0000-1600-000011000000}"/>
+    <hyperlink ref="D33" r:id="rId19" xr:uid="{00000000-0004-0000-1600-000012000000}"/>
+    <hyperlink ref="E33" r:id="rId20" xr:uid="{00000000-0004-0000-1600-000013000000}"/>
+    <hyperlink ref="E34" r:id="rId21" xr:uid="{00000000-0004-0000-1600-000014000000}"/>
+    <hyperlink ref="B34" r:id="rId22" xr:uid="{00000000-0004-0000-1600-000015000000}"/>
+    <hyperlink ref="C34" r:id="rId23" xr:uid="{00000000-0004-0000-1600-000016000000}"/>
+    <hyperlink ref="D34" r:id="rId24" xr:uid="{00000000-0004-0000-1600-000017000000}"/>
+    <hyperlink ref="B13" r:id="rId25" xr:uid="{00000000-0004-0000-1600-000018000000}"/>
+    <hyperlink ref="B17" r:id="rId26" xr:uid="{00000000-0004-0000-1600-000019000000}"/>
+    <hyperlink ref="C37" r:id="rId27" xr:uid="{1864C442-0D98-42E4-A5FA-B81EFAA05600}"/>
+    <hyperlink ref="B51" r:id="rId28" display="testersemail.278@gmail.com" xr:uid="{34BD3CEC-6340-4CBD-96DC-8D004250BF84}"/>
+    <hyperlink ref="C51" r:id="rId29" display="testersemail.278@gmail.com" xr:uid="{F1625DAF-2FCD-401E-B451-0BDE8A534010}"/>
+    <hyperlink ref="D51" r:id="rId30" display="testersemail.278@gmail.com" xr:uid="{07702DCB-4B62-4824-BB8A-83439182C0EA}"/>
+    <hyperlink ref="B52" r:id="rId31" display="testersemail.278@gmail.com" xr:uid="{5B1965CC-AC91-4E74-81AB-F5894D8C2D9D}"/>
+    <hyperlink ref="C52" r:id="rId32" display="testersemail.278@gmail.com" xr:uid="{41C8C86C-6596-41A3-B56B-A8BC6862F5E2}"/>
+    <hyperlink ref="D52" r:id="rId33" display="testersemail.278@gmail.com" xr:uid="{6A001A27-2D56-448C-93B5-920CBED417DB}"/>
+    <hyperlink ref="B53" r:id="rId34" display="testersemail.278@gmail.com" xr:uid="{E91B6625-1005-4D68-8C77-C24DDB033C2B}"/>
+    <hyperlink ref="C53" r:id="rId35" display="testersemail.278@gmail.com" xr:uid="{015DE811-F050-4B71-96A8-193BA2EE4365}"/>
+    <hyperlink ref="D53" r:id="rId36" display="testersemail.278@gmail.com" xr:uid="{6A56F90F-8F22-4C03-B66D-47272E68A409}"/>
+    <hyperlink ref="B56" r:id="rId37" display="testersemail.278@gmail.com" xr:uid="{6ECC3E7A-0650-471A-8118-361B581591B2}"/>
+    <hyperlink ref="C56" r:id="rId38" display="testersemail.278@gmail.com" xr:uid="{FFDC6FD4-A6DF-4655-B604-131C2FEC8FCA}"/>
+    <hyperlink ref="D56" r:id="rId39" display="testersemail.278@gmail.com" xr:uid="{E68CD518-C7DB-4D2A-BFE5-92473B1B7D82}"/>
+    <hyperlink ref="B57" r:id="rId40" display="testersemail.278@gmail.com" xr:uid="{C068F1CE-D006-4174-81C1-E2703766A79B}"/>
+    <hyperlink ref="C57" r:id="rId41" display="testersemail.278@gmail.com" xr:uid="{2393F234-B92D-48CB-B748-088EB5B8D9F0}"/>
+    <hyperlink ref="D57" r:id="rId42" display="testersemail.278@gmail.com" xr:uid="{EB4696D1-B300-4BCB-8F2F-4D7BB5228026}"/>
+    <hyperlink ref="B58" r:id="rId43" display="testersemail.278@gmail.com" xr:uid="{D584C792-57C6-4711-A589-420F8316183F}"/>
+    <hyperlink ref="C58" r:id="rId44" display="testersemail.278@gmail.com" xr:uid="{A41CA42C-EB84-484F-8296-5619531A4831}"/>
+    <hyperlink ref="D58" r:id="rId45" display="testersemail.278@gmail.com" xr:uid="{CEF795FF-332A-44D2-8EDF-ED7A85B34C63}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId43"/>
+  <pageSetup orientation="portrait" r:id="rId46"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Osprey EMEA E2E Testcases TEST_DGLD_OSP_CHE_FR_E2E_018 & 19 Changes Updated with Testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Osprey_EMEA/OSPEMEA_E2E_orderDetails.xlsx
+++ b/src/test/resources/TestData/Osprey_EMEA/OSPEMEA_E2E_orderDetails.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444DED5F-54C2-4514-AA40-212B4CCE0346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7CE359-340B-4828-B061-0B8EF2860957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="16" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Osprey_E2E" sheetId="26" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1835" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1835" uniqueCount="520">
   <si>
     <t>UserName</t>
   </si>
@@ -1622,6 +1622,9 @@
   </si>
   <si>
     <t>Standard Delivery (2-6 Days)</t>
+  </si>
+  <si>
+    <t>Consegna standard (2-7 giorni)</t>
   </si>
 </sst>
 </file>
@@ -2141,38 +2144,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB898B7-F8AD-4A5F-BE2F-C5B4C0E6C103}">
   <dimension ref="A1:AT48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="44.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="18" width="12.7109375" customWidth="1"/>
-    <col min="19" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="18" width="12.6640625" customWidth="1"/>
+    <col min="19" max="20" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11" bestFit="1" customWidth="1"/>
     <col min="26" max="31" width="11" customWidth="1"/>
-    <col min="38" max="38" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="23.42578125" customWidth="1"/>
-    <col min="45" max="45" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="23.44140625" customWidth="1"/>
+    <col min="45" max="45" width="23.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2312,7 +2315,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -2376,7 +2379,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>468</v>
       </c>
@@ -2431,7 +2434,7 @@
       <c r="AD3" s="5"/>
       <c r="AE3" s="5"/>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>467</v>
       </c>
@@ -2495,7 +2498,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="5" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -2519,7 +2522,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>463</v>
       </c>
@@ -2536,7 +2539,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>503</v>
       </c>
@@ -2553,7 +2556,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>461</v>
       </c>
@@ -2570,7 +2573,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>460</v>
       </c>
@@ -2587,7 +2590,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="10" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>457</v>
       </c>
@@ -2604,7 +2607,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>455</v>
       </c>
@@ -2621,7 +2624,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>454</v>
       </c>
@@ -2638,7 +2641,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>453</v>
       </c>
@@ -2655,7 +2658,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>452</v>
       </c>
@@ -2677,7 +2680,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>450</v>
       </c>
@@ -2699,7 +2702,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>94</v>
       </c>
@@ -2710,7 +2713,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>517</v>
       </c>
@@ -2719,7 +2722,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>383</v>
       </c>
@@ -2750,7 +2753,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>261</v>
       </c>
@@ -2761,7 +2764,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -2778,7 +2781,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>102</v>
       </c>
@@ -2798,7 +2801,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>104</v>
       </c>
@@ -2818,7 +2821,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>106</v>
       </c>
@@ -2838,7 +2841,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -2876,7 +2879,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>111</v>
       </c>
@@ -2917,7 +2920,7 @@
       <c r="AJ25" s="5"/>
       <c r="AK25" s="5"/>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>112</v>
       </c>
@@ -2934,7 +2937,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>141</v>
       </c>
@@ -2956,7 +2959,7 @@
       <c r="AH27" s="5"/>
       <c r="AI27" s="5"/>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>144</v>
       </c>
@@ -2990,7 +2993,7 @@
       <c r="T28" s="10"/>
       <c r="U28" s="10"/>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>146</v>
       </c>
@@ -3025,7 +3028,7 @@
       <c r="AD29" s="5"/>
       <c r="AE29" s="5"/>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>151</v>
       </c>
@@ -3087,7 +3090,7 @@
       <c r="AK30" s="5"/>
       <c r="AL30" s="7"/>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>156</v>
       </c>
@@ -3148,7 +3151,7 @@
       <c r="AF31" s="5"/>
       <c r="AG31" s="5"/>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>166</v>
       </c>
@@ -3166,7 +3169,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>178</v>
       </c>
@@ -3177,7 +3180,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>186</v>
       </c>
@@ -3197,7 +3200,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>91</v>
       </c>
@@ -3208,7 +3211,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>201</v>
       </c>
@@ -3225,7 +3228,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>203</v>
       </c>
@@ -3242,7 +3245,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>230</v>
       </c>
@@ -3259,7 +3262,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>253</v>
       </c>
@@ -3270,7 +3273,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>255</v>
       </c>
@@ -3281,7 +3284,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>256</v>
       </c>
@@ -3344,7 +3347,7 @@
       </c>
       <c r="AP41" s="7"/>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>115</v>
       </c>
@@ -3364,7 +3367,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>260</v>
       </c>
@@ -3375,7 +3378,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>268</v>
       </c>
@@ -3399,7 +3402,7 @@
       </c>
       <c r="U44" s="5"/>
     </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>271</v>
       </c>
@@ -3444,7 +3447,7 @@
       <c r="AH45" s="25"/>
       <c r="AI45" s="26"/>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>283</v>
       </c>
@@ -3452,7 +3455,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>432</v>
       </c>
@@ -3460,7 +3463,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>497</v>
       </c>
@@ -3546,12 +3549,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3614,7 +3617,7 @@
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -3638,7 +3641,7 @@
       <c r="S2" s="5"/>
       <c r="T2" s="7"/>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -3648,7 +3651,7 @@
       <c r="S3" s="5"/>
       <c r="T3" s="7"/>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>166</v>
       </c>
@@ -3667,7 +3670,7 @@
       <c r="S4" s="5"/>
       <c r="T4" s="7"/>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>97</v>
       </c>
@@ -3690,7 +3693,7 @@
       <c r="Q5" s="4"/>
       <c r="W5" s="5"/>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -3704,7 +3707,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>201</v>
       </c>
@@ -3732,12 +3735,12 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3775,7 +3778,7 @@
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>172</v>
       </c>
@@ -3793,27 +3796,27 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B3" s="10"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="H4" s="9"/>
       <c r="R4" s="5"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="H5" s="10"/>
       <c r="O5" s="3"/>
       <c r="P5" s="4"/>
       <c r="V5" s="5"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="H6" s="5"/>
     </row>
   </sheetData>
@@ -3830,9 +3833,9 @@
       <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3897,7 +3900,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -3935,7 +3938,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -3943,7 +3946,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>201</v>
       </c>
@@ -3957,7 +3960,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>106</v>
       </c>
@@ -3971,7 +3974,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>94</v>
       </c>
@@ -3998,16 +4001,16 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
     <col min="15" max="17" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4084,7 +4087,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -4122,7 +4125,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -4145,7 +4148,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>166</v>
       </c>
@@ -4156,7 +4159,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -4167,7 +4170,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>201</v>
       </c>
@@ -4198,19 +4201,19 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4293,7 +4296,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -4334,7 +4337,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -4354,7 +4357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -4386,7 +4389,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>128</v>
       </c>
@@ -4400,7 +4403,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>134</v>
       </c>
@@ -4429,13 +4432,13 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4464,7 +4467,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -4484,7 +4487,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>215</v>
       </c>
@@ -4492,7 +4495,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>216</v>
       </c>
@@ -4517,13 +4520,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4536,7 +4539,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -4564,23 +4567,23 @@
       <selection activeCell="I2" sqref="I2:M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4648,7 +4651,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -4689,7 +4692,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -4715,7 +4718,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -4735,7 +4738,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>136</v>
       </c>
@@ -4761,7 +4764,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="195" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>137</v>
       </c>
@@ -4790,7 +4793,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="N7" s="15"/>
     </row>
   </sheetData>
@@ -4809,21 +4812,21 @@
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="44.7109375" customWidth="1"/>
+    <col min="14" max="14" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="44.6640625" customWidth="1"/>
     <col min="16" max="16" width="22" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4897,7 +4900,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -4938,7 +4941,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>139</v>
       </c>
@@ -4961,7 +4964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>201</v>
       </c>
@@ -4991,13 +4994,13 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="222.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="222.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5049,7 +5052,7 @@
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>304</v>
       </c>
@@ -5057,7 +5060,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>305</v>
       </c>
@@ -5089,7 +5092,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>306</v>
       </c>
@@ -5117,19 +5120,19 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5173,7 +5176,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -5187,7 +5190,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -5202,7 +5205,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -5212,63 +5215,63 @@
         <v>386</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D12" s="8"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="G14" s="6"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E21" s="2"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D22" s="9"/>
       <c r="E22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
     </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
     </row>
@@ -5289,16 +5292,16 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="13" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="13" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5345,7 +5348,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -5372,7 +5375,7 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>162</v>
       </c>
@@ -5383,7 +5386,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>323</v>
       </c>
@@ -5433,24 +5436,24 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" customWidth="1"/>
-    <col min="18" max="18" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5546875" customWidth="1"/>
+    <col min="18" max="18" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5523,7 +5526,7 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -5562,7 +5565,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -5579,7 +5582,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>166</v>
       </c>
@@ -5591,7 +5594,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -5599,7 +5602,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>190</v>
       </c>
@@ -5616,7 +5619,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>192</v>
       </c>
@@ -5624,7 +5627,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>201</v>
       </c>
@@ -5638,7 +5641,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -5649,7 +5652,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>379</v>
       </c>
@@ -5676,15 +5679,15 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5827,7 +5830,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>334</v>
       </c>
@@ -5898,7 +5901,7 @@
         <v>32881</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>314</v>
       </c>
@@ -5959,17 +5962,17 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -6037,7 +6040,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -6059,7 +6062,7 @@
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>198</v>
       </c>
@@ -6088,40 +6091,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:AT64"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="AE10" sqref="AE10"/>
+      <selection pane="bottomLeft" activeCell="AJ6" sqref="AJ6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="44.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="12.7109375" customWidth="1"/>
-    <col min="18" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="12.6640625" customWidth="1"/>
+    <col min="18" max="19" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
     <col min="25" max="30" width="11" customWidth="1"/>
-    <col min="31" max="31" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="23.42578125" customWidth="1"/>
-    <col min="43" max="43" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="23.44140625" customWidth="1"/>
+    <col min="43" max="43" width="23.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -6261,7 +6264,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -6324,7 +6327,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -6347,7 +6350,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -6358,7 +6361,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>487</v>
       </c>
@@ -6367,16 +6370,16 @@
         <v>488</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>495</v>
       </c>
       <c r="M6" s="2"/>
       <c r="AJ6" s="5" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>383</v>
       </c>
@@ -6406,7 +6409,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>261</v>
       </c>
@@ -6417,7 +6420,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -6434,7 +6437,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>102</v>
       </c>
@@ -6451,7 +6454,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>104</v>
       </c>
@@ -6468,7 +6471,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>106</v>
       </c>
@@ -6485,7 +6488,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -6520,7 +6523,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>111</v>
       </c>
@@ -6561,7 +6564,7 @@
       <c r="AH14" s="5"/>
       <c r="AI14" s="5"/>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>112</v>
       </c>
@@ -6578,7 +6581,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>141</v>
       </c>
@@ -6597,7 +6600,7 @@
       <c r="AF16" s="5"/>
       <c r="AG16" s="5"/>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>508</v>
       </c>
@@ -6614,7 +6617,7 @@
       <c r="AF17" s="5"/>
       <c r="AG17" s="5"/>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>144</v>
       </c>
@@ -6647,7 +6650,7 @@
       <c r="S18" s="10"/>
       <c r="T18" s="10"/>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>146</v>
       </c>
@@ -6682,7 +6685,7 @@
       <c r="AC19" s="5"/>
       <c r="AD19" s="5"/>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>151</v>
       </c>
@@ -6743,7 +6746,7 @@
       <c r="AI20" s="5"/>
       <c r="AJ20" s="7"/>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>156</v>
       </c>
@@ -6802,7 +6805,7 @@
       <c r="AD21" s="5"/>
       <c r="AE21" s="5"/>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>166</v>
       </c>
@@ -6817,7 +6820,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>178</v>
       </c>
@@ -6828,7 +6831,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>186</v>
       </c>
@@ -6848,7 +6851,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>91</v>
       </c>
@@ -6859,7 +6862,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>201</v>
       </c>
@@ -6876,7 +6879,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>203</v>
       </c>
@@ -6893,7 +6896,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>230</v>
       </c>
@@ -6910,7 +6913,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>253</v>
       </c>
@@ -6921,7 +6924,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>255</v>
       </c>
@@ -6932,7 +6935,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>256</v>
       </c>
@@ -6994,7 +6997,7 @@
       </c>
       <c r="AN31" s="7"/>
     </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>115</v>
       </c>
@@ -7014,7 +7017,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>260</v>
       </c>
@@ -7025,7 +7028,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>268</v>
       </c>
@@ -7049,7 +7052,7 @@
       </c>
       <c r="T34" s="5"/>
     </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>271</v>
       </c>
@@ -7094,7 +7097,7 @@
       <c r="AF35" s="25"/>
       <c r="AG35" s="26"/>
     </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>230</v>
       </c>
@@ -7102,7 +7105,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>222</v>
       </c>
@@ -7113,7 +7116,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>224</v>
       </c>
@@ -7138,7 +7141,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="39" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:46" ht="60" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>399</v>
       </c>
@@ -7156,7 +7159,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:46" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:46" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>489</v>
       </c>
@@ -7177,7 +7180,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:46" ht="60" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>423</v>
       </c>
@@ -7195,7 +7198,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="42" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:46" ht="30" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>402</v>
       </c>
@@ -7209,7 +7212,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>477</v>
       </c>
@@ -7226,7 +7229,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>485</v>
       </c>
@@ -7235,7 +7238,7 @@
       </c>
       <c r="AI44" s="5"/>
     </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>476</v>
       </c>
@@ -7246,7 +7249,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="46" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:46" ht="30" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>391</v>
       </c>
@@ -7260,7 +7263,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="47" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:46" ht="60" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>413</v>
       </c>
@@ -7274,7 +7277,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:46" ht="30" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>418</v>
       </c>
@@ -7288,7 +7291,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:41" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:41" ht="30" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>419</v>
       </c>
@@ -7302,7 +7305,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="50" spans="1:41" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:41" ht="60" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>420</v>
       </c>
@@ -7316,7 +7319,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="51" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:41" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>427</v>
       </c>
@@ -7330,7 +7333,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="52" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>392</v>
       </c>
@@ -7365,7 +7368,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>407</v>
       </c>
@@ -7400,7 +7403,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>408</v>
       </c>
@@ -7435,7 +7438,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="55" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:41" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>401</v>
       </c>
@@ -7443,7 +7446,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="56" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:41" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>432</v>
       </c>
@@ -7451,7 +7454,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="57" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:41" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>504</v>
       </c>
@@ -7459,7 +7462,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="58" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:41" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>506</v>
       </c>
@@ -7467,7 +7470,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="59" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:41" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>511</v>
       </c>
@@ -7475,7 +7478,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="60" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:41" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>513</v>
       </c>
@@ -7483,7 +7486,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="61" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:41" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>515</v>
       </c>
@@ -7491,7 +7494,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="62" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>421</v>
       </c>
@@ -7526,7 +7529,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="63" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>478</v>
       </c>
@@ -7561,7 +7564,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="64" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>490</v>
       </c>
@@ -7598,10 +7601,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-1600-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-1600-000000000000}"/>
     <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-1600-000001000000}"/>
     <hyperlink ref="F2" r:id="rId3" display="Testers@278" xr:uid="{00000000-0004-0000-1600-000002000000}"/>
-    <hyperlink ref="C2" r:id="rId4" display="lotusqa.gld.stg.os.us.automation.01@gmail.com" xr:uid="{00000000-0004-0000-1600-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-1600-000003000000}"/>
     <hyperlink ref="E13" r:id="rId5" xr:uid="{00000000-0004-0000-1600-000004000000}"/>
     <hyperlink ref="C14" r:id="rId6" xr:uid="{00000000-0004-0000-1600-000005000000}"/>
     <hyperlink ref="C18" r:id="rId7" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-1600-000007000000}"/>
@@ -7611,7 +7614,7 @@
     <hyperlink ref="B21" r:id="rId11" xr:uid="{00000000-0004-0000-1600-00000B000000}"/>
     <hyperlink ref="C21" r:id="rId12" xr:uid="{00000000-0004-0000-1600-00000C000000}"/>
     <hyperlink ref="C31" r:id="rId13" xr:uid="{00000000-0004-0000-1600-00000D000000}"/>
-    <hyperlink ref="D2" r:id="rId14" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-1600-00000E000000}"/>
+    <hyperlink ref="D2" r:id="rId14" xr:uid="{00000000-0004-0000-1600-00000E000000}"/>
     <hyperlink ref="L32" r:id="rId15" display="testersemail.278@gmail.com" xr:uid="{00000000-0004-0000-1600-00000F000000}"/>
     <hyperlink ref="B34" r:id="rId16" xr:uid="{00000000-0004-0000-1600-000010000000}"/>
     <hyperlink ref="C34" r:id="rId17" xr:uid="{00000000-0004-0000-1600-000011000000}"/>
@@ -7659,23 +7662,23 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="24.7109375" customWidth="1"/>
-    <col min="13" max="13" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="24.6640625" customWidth="1"/>
+    <col min="13" max="13" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.7109375" customWidth="1"/>
+    <col min="15" max="15" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -7800,7 +7803,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -7852,7 +7855,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>220</v>
       </c>
@@ -7884,7 +7887,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -7892,7 +7895,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -7906,7 +7909,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -7941,7 +7944,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -7955,7 +7958,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -7969,7 +7972,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -8004,7 +8007,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>141</v>
       </c>
@@ -8020,7 +8023,7 @@
       <c r="AB10" s="5"/>
       <c r="AC10" s="5"/>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>144</v>
       </c>
@@ -8050,7 +8053,7 @@
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>146</v>
       </c>
@@ -8076,7 +8079,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>166</v>
       </c>
@@ -8091,7 +8094,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>178</v>
       </c>
@@ -8099,7 +8102,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>186</v>
       </c>
@@ -8116,7 +8119,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>91</v>
       </c>
@@ -8124,7 +8127,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>201</v>
       </c>
@@ -8138,7 +8141,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>203</v>
       </c>
@@ -8161,7 +8164,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>222</v>
       </c>
@@ -8172,7 +8175,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>224</v>
       </c>
@@ -8191,7 +8194,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>231</v>
       </c>
@@ -8202,7 +8205,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>292</v>
       </c>
@@ -8216,7 +8219,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>230</v>
       </c>
@@ -8236,7 +8239,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>283</v>
       </c>
@@ -8250,7 +8253,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>234</v>
       </c>
@@ -8258,7 +8261,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>235</v>
       </c>
@@ -8266,7 +8269,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>89</v>
       </c>
@@ -8286,7 +8289,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>268</v>
       </c>
@@ -8336,33 +8339,33 @@
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="154.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="42.7109375" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" customWidth="1"/>
-    <col min="12" max="12" width="30.5703125" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" customWidth="1"/>
-    <col min="14" max="15" width="22.28515625" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="154.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.6640625" customWidth="1"/>
+    <col min="11" max="11" width="30.6640625" customWidth="1"/>
+    <col min="12" max="12" width="30.5546875" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" customWidth="1"/>
+    <col min="14" max="15" width="22.33203125" customWidth="1"/>
+    <col min="16" max="16" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.28515625" customWidth="1"/>
+    <col min="22" max="22" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -8420,7 +8423,7 @@
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -8440,7 +8443,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -8451,7 +8454,7 @@
       <c r="T3" s="5"/>
       <c r="U3" s="7"/>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -8462,7 +8465,7 @@
       <c r="T4" s="5"/>
       <c r="U4" s="7"/>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -8476,7 +8479,7 @@
       <c r="R5" s="4"/>
       <c r="X5" s="5"/>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -8487,7 +8490,7 @@
       <c r="R6" s="4"/>
       <c r="X6" s="5"/>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -8501,7 +8504,7 @@
       <c r="R7" s="4"/>
       <c r="X7" s="5"/>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -8511,7 +8514,7 @@
       <c r="K8" s="2"/>
       <c r="X8" s="5"/>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>355</v>
       </c>
@@ -8525,7 +8528,7 @@
       </c>
       <c r="X9" s="5"/>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>356</v>
       </c>
@@ -8539,7 +8542,7 @@
       </c>
       <c r="X10" s="5"/>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>359</v>
       </c>
@@ -8550,7 +8553,7 @@
       <c r="K11" s="2"/>
       <c r="X11" s="5"/>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>366</v>
       </c>
@@ -8565,13 +8568,13 @@
       <c r="K12" s="2"/>
       <c r="AF12" s="10"/>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="X13" s="5"/>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -8579,22 +8582,22 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="T15" s="5"/>
       <c r="U15" s="7"/>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="T16" s="5"/>
       <c r="U16" s="7"/>
     </row>
-    <row r="17" spans="4:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:31" x14ac:dyDescent="0.3">
       <c r="T17" s="5"/>
       <c r="U17" s="7"/>
     </row>
-    <row r="18" spans="4:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:31" x14ac:dyDescent="0.3">
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -8605,22 +8608,22 @@
       <c r="U18" s="7"/>
       <c r="AE18" s="5"/>
     </row>
-    <row r="19" spans="4:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:31" x14ac:dyDescent="0.3">
       <c r="T19" s="5"/>
       <c r="U19" s="7"/>
       <c r="V19" s="5"/>
     </row>
-    <row r="20" spans="4:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:31" x14ac:dyDescent="0.3">
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
     </row>
-    <row r="21" spans="4:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:31" x14ac:dyDescent="0.3">
       <c r="F21" s="2"/>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
     </row>
-    <row r="22" spans="4:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="2"/>
@@ -8630,18 +8633,18 @@
       <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
     </row>
-    <row r="23" spans="4:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:31" x14ac:dyDescent="0.3">
       <c r="Q23" s="5"/>
       <c r="R23" s="5"/>
     </row>
-    <row r="26" spans="4:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:31" x14ac:dyDescent="0.3">
       <c r="I26" s="10"/>
       <c r="J26" s="10"/>
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
       <c r="O26" s="5"/>
     </row>
-    <row r="27" spans="4:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:31" x14ac:dyDescent="0.3">
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
@@ -8660,18 +8663,18 @@
       <selection activeCell="AC9" sqref="AC9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.7109375" customWidth="1"/>
-    <col min="35" max="35" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.6640625" customWidth="1"/>
+    <col min="35" max="35" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -8781,7 +8784,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -8814,7 +8817,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -8828,7 +8831,7 @@
       <c r="S3" s="5"/>
       <c r="T3" s="7"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -8843,7 +8846,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -8860,7 +8863,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -8874,7 +8877,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>167</v>
       </c>
@@ -8894,7 +8897,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>169</v>
       </c>
@@ -8908,7 +8911,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>182</v>
       </c>
@@ -8948,18 +8951,18 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -8985,7 +8988,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -8997,7 +9000,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -9040,23 +9043,23 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="15" width="25.140625" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="139.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="15" width="25.109375" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="139.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9127,7 +9130,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -9155,7 +9158,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -9164,7 +9167,7 @@
       </c>
       <c r="W3" s="5"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>89</v>
       </c>
@@ -9181,7 +9184,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -9189,7 +9192,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>146</v>
       </c>
@@ -9218,7 +9221,7 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>147</v>
       </c>
@@ -9247,7 +9250,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -9261,7 +9264,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>162</v>
       </c>
@@ -9275,10 +9278,10 @@
         <v>163</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V12" s="9"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="U15" s="9"/>
     </row>
   </sheetData>
@@ -9303,15 +9306,15 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9382,7 +9385,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -9430,7 +9433,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -9479,7 +9482,7 @@
       </c>
       <c r="W3" s="9"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -9530,7 +9533,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -9554,7 +9557,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -9571,7 +9574,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -9607,28 +9610,28 @@
       <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="22" bestFit="1" customWidth="1"/>
     <col min="18" max="20" width="22" customWidth="1"/>
-    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9705,7 +9708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -9747,7 +9750,7 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -9767,7 +9770,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -9775,7 +9778,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>106</v>
       </c>
@@ -9789,7 +9792,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -9812,7 +9815,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>146</v>
       </c>
@@ -9842,7 +9845,7 @@
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>166</v>
       </c>
@@ -9854,7 +9857,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>201</v>
       </c>
@@ -9871,7 +9874,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>381</v>
       </c>
@@ -9920,18 +9923,18 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9957,7 +9960,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -9974,12 +9977,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>89</v>
       </c>
@@ -9990,7 +9993,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>97</v>
       </c>
@@ -10005,7 +10008,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H9" s="9"/>
     </row>
   </sheetData>

</xml_diff>